<commit_message>
Added code for atoi
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CBC844-619E-495E-A3FA-857AA1411B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194056DA-5B98-478C-B912-66F5B52B721C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="141">
   <si>
     <t>ID</t>
   </si>
@@ -442,6 +442,18 @@
   </si>
   <si>
     <t>Recursion, Pattern Based</t>
+  </si>
+  <si>
+    <t>String to int (Atoi)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/string-to-integer-atoi/description/</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Recursion, Edge Cases</t>
   </si>
 </sst>
 </file>
@@ -477,7 +489,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -532,6 +544,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -546,7 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -557,11 +575,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -867,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -952,17 +971,17 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -983,15 +1002,15 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1012,15 +1031,15 @@
       <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -1041,15 +1060,15 @@
       <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1073,15 +1092,15 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1102,15 +1121,15 @@
       <c r="G8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1134,15 +1153,15 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1166,15 +1185,15 @@
       <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1198,15 +1217,15 @@
       <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -1227,15 +1246,15 @@
       <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1259,15 +1278,15 @@
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -1291,15 +1310,15 @@
       <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -1323,15 +1342,15 @@
       <c r="G15" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -1355,15 +1374,15 @@
       <c r="G16" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
@@ -1387,15 +1406,15 @@
       <c r="G17" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
@@ -1416,15 +1435,15 @@
       <c r="G18" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
@@ -1448,15 +1467,15 @@
       <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
@@ -1477,15 +1496,15 @@
       <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
@@ -1509,15 +1528,15 @@
       <c r="G21" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22">
@@ -1541,15 +1560,15 @@
       <c r="G22" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23">
@@ -1570,15 +1589,15 @@
       <c r="G23" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24">
@@ -1599,15 +1618,15 @@
       <c r="G24" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25">
@@ -1628,15 +1647,15 @@
       <c r="G25" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26">
@@ -1660,15 +1679,15 @@
       <c r="G26" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27">
@@ -1692,15 +1711,15 @@
       <c r="G27" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28">
@@ -1724,15 +1743,15 @@
       <c r="G28" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29">
@@ -1756,15 +1775,15 @@
       <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30">
@@ -1788,15 +1807,15 @@
       <c r="G30" t="s">
         <v>74</v>
       </c>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31">
@@ -1817,15 +1836,15 @@
       <c r="G31" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32">
@@ -1849,15 +1868,15 @@
       <c r="G32" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33">
@@ -1881,15 +1900,15 @@
       <c r="G33" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34">
@@ -1913,15 +1932,15 @@
       <c r="G34" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35">
@@ -1945,15 +1964,15 @@
       <c r="G35" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36">
@@ -2132,10 +2151,10 @@
       <c r="C43">
         <v>50</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="11" t="s">
         <v>135</v>
       </c>
       <c r="F43" t="s">
@@ -2149,6 +2168,35 @@
       </c>
       <c r="I43" s="8">
         <v>46037</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F44" t="s">
+        <v>140</v>
+      </c>
+      <c r="G44" t="s">
+        <v>131</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="I44" s="8">
+        <v>46033</v>
       </c>
     </row>
     <row r="54" spans="9:9" x14ac:dyDescent="0.35">
@@ -3033,6 +3081,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D43" r:id="rId1" xr:uid="{41F2C050-F050-4E69-AC4B-AA74BBE1DE7D}"/>
+    <hyperlink ref="D44" r:id="rId2" xr:uid="{9F5FE31E-3EDF-4BA8-BDC5-47DB1805E96A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added code for daily leetcode challenge day 8 and 9
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194056DA-5B98-478C-B912-66F5B52B721C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63691A4-F989-4A39-AF1C-A6974D72D37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="143">
   <si>
     <t>ID</t>
   </si>
@@ -454,6 +454,12 @@
   </si>
   <si>
     <t>Recursion, Edge Cases</t>
+  </si>
+  <si>
+    <t>Good Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-good-numbers/</t>
   </si>
 </sst>
 </file>
@@ -577,10 +583,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -887,7 +893,7 @@
   <dimension ref="A1:R199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,17 +977,17 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1002,15 +1008,15 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1031,15 +1037,15 @@
       <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -1060,15 +1066,15 @@
       <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1092,15 +1098,15 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1121,15 +1127,15 @@
       <c r="G8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1153,15 +1159,15 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1185,15 +1191,15 @@
       <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1217,15 +1223,15 @@
       <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -1246,15 +1252,15 @@
       <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1278,15 +1284,15 @@
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -1310,15 +1316,15 @@
       <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -1342,15 +1348,15 @@
       <c r="G15" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -1374,15 +1380,15 @@
       <c r="G16" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
@@ -1406,15 +1412,15 @@
       <c r="G17" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
@@ -1435,15 +1441,15 @@
       <c r="G18" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
@@ -1467,15 +1473,15 @@
       <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
@@ -1496,15 +1502,15 @@
       <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="12"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
@@ -1528,15 +1534,15 @@
       <c r="G21" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22">
@@ -1560,15 +1566,15 @@
       <c r="G22" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23">
@@ -1589,15 +1595,15 @@
       <c r="G23" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24">
@@ -1618,15 +1624,15 @@
       <c r="G24" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25">
@@ -1647,15 +1653,15 @@
       <c r="G25" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26">
@@ -1679,15 +1685,15 @@
       <c r="G26" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27">
@@ -1711,15 +1717,15 @@
       <c r="G27" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28">
@@ -1743,15 +1749,15 @@
       <c r="G28" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29">
@@ -1775,15 +1781,15 @@
       <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="12"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30">
@@ -1807,15 +1813,15 @@
       <c r="G30" t="s">
         <v>74</v>
       </c>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="12"/>
-      <c r="R30" s="12"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31">
@@ -1836,15 +1842,15 @@
       <c r="G31" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32">
@@ -1868,15 +1874,15 @@
       <c r="G32" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="12"/>
-      <c r="R32" s="12"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33">
@@ -1900,15 +1906,15 @@
       <c r="G33" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="12"/>
-      <c r="R33" s="12"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34">
@@ -1932,15 +1938,15 @@
       <c r="G34" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="12"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35">
@@ -1964,15 +1970,15 @@
       <c r="G35" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="12"/>
-      <c r="R35" s="12"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36">
@@ -2183,7 +2189,7 @@
       <c r="D44" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="11" t="s">
         <v>135</v>
       </c>
       <c r="F44" t="s">
@@ -2192,11 +2198,40 @@
       <c r="G44" t="s">
         <v>131</v>
       </c>
-      <c r="H44" s="13" t="s">
+      <c r="H44" s="12" t="s">
         <v>139</v>
       </c>
       <c r="I44" s="8">
         <v>46033</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45">
+        <v>1922</v>
+      </c>
+      <c r="D45" t="s">
+        <v>142</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F45" t="s">
+        <v>136</v>
+      </c>
+      <c r="G45" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I45" s="8">
+        <v>46037</v>
       </c>
     </row>
     <row r="54" spans="9:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added code for reverse a stack
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63691A4-F989-4A39-AF1C-A6974D72D37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4135CCD-0C67-4C33-BC1A-8B8F858A84A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="146">
   <si>
     <t>ID</t>
   </si>
@@ -460,6 +460,15 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/count-good-numbers/</t>
+  </si>
+  <si>
+    <t>Sort a stack</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/sort-a-stack</t>
+  </si>
+  <si>
+    <t>Recursion, traverse</t>
   </si>
 </sst>
 </file>
@@ -893,7 +902,7 @@
   <dimension ref="A1:R199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2234,6 +2243,32 @@
         <v>46037</v>
       </c>
     </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F46" t="s">
+        <v>145</v>
+      </c>
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I46" s="8">
+        <v>46033</v>
+      </c>
+    </row>
     <row r="54" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I54" t="str">
         <f>IF(H54="Hard",#REF!+ 3,IF(H54="Medium",#REF!+ 7,IF(H54="Easy",#REF!+ 30,"")))</f>
@@ -3117,6 +3152,7 @@
   <hyperlinks>
     <hyperlink ref="D43" r:id="rId1" xr:uid="{41F2C050-F050-4E69-AC4B-AA74BBE1DE7D}"/>
     <hyperlink ref="D44" r:id="rId2" xr:uid="{9F5FE31E-3EDF-4BA8-BDC5-47DB1805E96A}"/>
+    <hyperlink ref="D46" r:id="rId3" xr:uid="{6EF8B0EF-27B5-4A6C-8FAA-8D8FFF890651}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added most optimised solution for move zeroes
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4135CCD-0C67-4C33-BC1A-8B8F858A84A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D5C602-E03A-471E-A61E-3DEC65C7266C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA Tracker" sheetId="1" r:id="rId1"/>
+    <sheet name="Practice Previous" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="152">
   <si>
     <t>ID</t>
   </si>
@@ -469,6 +470,24 @@
   </si>
   <si>
     <t>Recursion, traverse</t>
+  </si>
+  <si>
+    <t>Reverse a stack</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/reverse-a-stack</t>
+  </si>
+  <si>
+    <t>Move Zeroes</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/move-zeroes/description/</t>
+  </si>
+  <si>
+    <t>2-Pointer</t>
+  </si>
+  <si>
+    <t>Easy</t>
   </si>
 </sst>
 </file>
@@ -504,7 +523,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +584,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -579,7 +604,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -596,6 +621,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -901,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2269,6 +2296,32 @@
         <v>46033</v>
       </c>
     </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>146</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F47" t="s">
+        <v>145</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I47" s="8">
+        <v>46037</v>
+      </c>
+    </row>
     <row r="54" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I54" t="str">
         <f>IF(H54="Hard",#REF!+ 3,IF(H54="Medium",#REF!+ 7,IF(H54="Easy",#REF!+ 30,"")))</f>
@@ -3153,7 +3206,89 @@
     <hyperlink ref="D43" r:id="rId1" xr:uid="{41F2C050-F050-4E69-AC4B-AA74BBE1DE7D}"/>
     <hyperlink ref="D44" r:id="rId2" xr:uid="{9F5FE31E-3EDF-4BA8-BDC5-47DB1805E96A}"/>
     <hyperlink ref="D46" r:id="rId3" xr:uid="{6EF8B0EF-27B5-4A6C-8FAA-8D8FFF890651}"/>
+    <hyperlink ref="D47" r:id="rId4" xr:uid="{33F92BC2-1EF1-499C-BFC6-6432476C5EF5}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2">
+        <v>283</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2" s="15">
+        <v>46052</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{446E0945-919F-4C75-A7DF-820B86BF045D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added daily coding challenge for day 10
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D5C602-E03A-471E-A61E-3DEC65C7266C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E85083-A90E-4085-A5EB-9F5351CCB73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA Tracker" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="156">
   <si>
     <t>ID</t>
   </si>
@@ -488,6 +488,18 @@
   </si>
   <si>
     <t>Easy</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/generate-binary-strings-without-consecutive-1s</t>
+  </si>
+  <si>
+    <t>Generate Binary Number</t>
+  </si>
+  <si>
+    <t>Generate all parentheses</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/generate-parentheses/description/</t>
   </si>
 </sst>
 </file>
@@ -604,7 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -618,11 +630,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -928,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1013,17 +1026,17 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1044,15 +1057,15 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1073,15 +1086,15 @@
       <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -1102,15 +1115,15 @@
       <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1134,15 +1147,15 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1163,15 +1176,15 @@
       <c r="G8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1195,15 +1208,15 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1227,15 +1240,15 @@
       <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1259,15 +1272,15 @@
       <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -1288,15 +1301,15 @@
       <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1320,15 +1333,15 @@
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -1352,15 +1365,15 @@
       <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -1384,15 +1397,15 @@
       <c r="G15" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -1416,15 +1429,15 @@
       <c r="G16" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
@@ -1448,15 +1461,15 @@
       <c r="G17" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
@@ -1477,15 +1490,15 @@
       <c r="G18" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
@@ -1509,15 +1522,15 @@
       <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
@@ -1538,15 +1551,15 @@
       <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
@@ -1570,15 +1583,15 @@
       <c r="G21" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22">
@@ -1602,15 +1615,15 @@
       <c r="G22" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23">
@@ -1631,15 +1644,15 @@
       <c r="G23" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24">
@@ -1660,15 +1673,15 @@
       <c r="G24" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25">
@@ -1689,15 +1702,15 @@
       <c r="G25" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26">
@@ -1721,15 +1734,15 @@
       <c r="G26" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27">
@@ -1753,15 +1766,15 @@
       <c r="G27" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28">
@@ -1785,15 +1798,15 @@
       <c r="G28" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29">
@@ -1817,15 +1830,15 @@
       <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30">
@@ -1849,15 +1862,15 @@
       <c r="G30" t="s">
         <v>74</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31">
@@ -1878,15 +1891,15 @@
       <c r="G31" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32">
@@ -1910,15 +1923,15 @@
       <c r="G32" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33">
@@ -1942,15 +1955,15 @@
       <c r="G33" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34">
@@ -1974,15 +1987,15 @@
       <c r="G34" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35">
@@ -2006,15 +2019,15 @@
       <c r="G35" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36">
@@ -2322,67 +2335,122 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F48" t="s">
+        <v>135</v>
+      </c>
+      <c r="G48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I48" s="16">
+        <v>46034</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>155</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F49" t="s">
+        <v>135</v>
+      </c>
+      <c r="G49" t="s">
+        <v>131</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I49" s="8">
+        <v>46038</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I54" t="str">
         <f>IF(H54="Hard",#REF!+ 3,IF(H54="Medium",#REF!+ 7,IF(H54="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I55" t="str">
         <f>IF(H55="Hard",#REF!+ 3,IF(H55="Medium",#REF!+ 7,IF(H55="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I56" t="str">
         <f>IF(H56="Hard",#REF!+ 3,IF(H56="Medium",#REF!+ 7,IF(H56="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I57" t="str">
         <f>IF(H57="Hard",#REF!+ 3,IF(H57="Medium",#REF!+ 7,IF(H57="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I58" t="str">
         <f>IF(H58="Hard",#REF!+ 3,IF(H58="Medium",#REF!+ 7,IF(H58="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I59" t="str">
         <f>IF(H59="Hard",#REF!+ 3,IF(H59="Medium",#REF!+ 7,IF(H59="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I60" t="str">
         <f>IF(H60="Hard",#REF!+ 3,IF(H60="Medium",#REF!+ 7,IF(H60="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I61" t="str">
         <f>IF(H61="Hard",#REF!+ 3,IF(H61="Medium",#REF!+ 7,IF(H61="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I62" t="str">
         <f>IF(H62="Hard",#REF!+ 3,IF(H62="Medium",#REF!+ 7,IF(H62="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I63" t="str">
         <f>IF(H63="Hard",#REF!+ 3,IF(H63="Medium",#REF!+ 7,IF(H63="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I64" t="str">
         <f>IF(H64="Hard",#REF!+ 3,IF(H64="Medium",#REF!+ 7,IF(H64="Easy",#REF!+ 30,"")))</f>
         <v/>
@@ -3207,6 +3275,7 @@
     <hyperlink ref="D44" r:id="rId2" xr:uid="{9F5FE31E-3EDF-4BA8-BDC5-47DB1805E96A}"/>
     <hyperlink ref="D46" r:id="rId3" xr:uid="{6EF8B0EF-27B5-4A6C-8FAA-8D8FFF890651}"/>
     <hyperlink ref="D47" r:id="rId4" xr:uid="{33F92BC2-1EF1-499C-BFC6-6432476C5EF5}"/>
+    <hyperlink ref="D48" r:id="rId5" xr:uid="{F67762AC-77CD-4EF5-AC97-5E4313FB66FA}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3216,7 +3285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -3278,10 +3347,10 @@
       <c r="G2" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="14">
         <v>46052</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added code for daily challenge day 11
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E85083-A90E-4085-A5EB-9F5351CCB73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EC075B-55EF-4863-852F-C311BF54639F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -632,10 +632,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -942,7 +942,7 @@
   <dimension ref="A1:R199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1026,17 +1026,17 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1057,15 +1057,15 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1086,15 +1086,15 @@
       <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -1115,15 +1115,15 @@
       <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1147,15 +1147,15 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1176,15 +1176,15 @@
       <c r="G8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1208,15 +1208,15 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1240,15 +1240,15 @@
       <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1272,15 +1272,15 @@
       <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -1301,15 +1301,15 @@
       <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1333,15 +1333,15 @@
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -1365,15 +1365,15 @@
       <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -1397,15 +1397,15 @@
       <c r="G15" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -1429,15 +1429,15 @@
       <c r="G16" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
@@ -1461,15 +1461,15 @@
       <c r="G17" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
@@ -1490,15 +1490,15 @@
       <c r="G18" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
@@ -1522,15 +1522,15 @@
       <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
@@ -1551,15 +1551,15 @@
       <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
@@ -1583,15 +1583,15 @@
       <c r="G21" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22">
@@ -1615,15 +1615,15 @@
       <c r="G22" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23">
@@ -1644,15 +1644,15 @@
       <c r="G23" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24">
@@ -1673,15 +1673,15 @@
       <c r="G24" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25">
@@ -1702,15 +1702,15 @@
       <c r="G25" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26">
@@ -1734,15 +1734,15 @@
       <c r="G26" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27">
@@ -1766,15 +1766,15 @@
       <c r="G27" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28">
@@ -1798,15 +1798,15 @@
       <c r="G28" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29">
@@ -1830,15 +1830,15 @@
       <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30">
@@ -1862,15 +1862,15 @@
       <c r="G30" t="s">
         <v>74</v>
       </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31">
@@ -1891,15 +1891,15 @@
       <c r="G31" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32">
@@ -1923,15 +1923,15 @@
       <c r="G32" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33">
@@ -1955,15 +1955,15 @@
       <c r="G33" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34">
@@ -1987,15 +1987,15 @@
       <c r="G34" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35">
@@ -2019,15 +2019,15 @@
       <c r="G35" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36">
@@ -2247,11 +2247,11 @@
       <c r="G44" t="s">
         <v>131</v>
       </c>
-      <c r="H44" s="12" t="s">
-        <v>139</v>
+      <c r="H44" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="I44" s="8">
-        <v>46033</v>
+        <v>46039</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.35">
@@ -2306,7 +2306,7 @@
         <v>139</v>
       </c>
       <c r="I46" s="8">
-        <v>46033</v>
+        <v>46035</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
@@ -2357,7 +2357,7 @@
       <c r="H48" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="I48" s="16">
+      <c r="I48" s="15">
         <v>46034</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added code for all subsets
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EC075B-55EF-4863-852F-C311BF54639F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA9816A-5FC9-4E77-9CA0-010EFDF52466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA Tracker" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="180">
   <si>
     <t>ID</t>
   </si>
@@ -500,6 +500,78 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/description/</t>
+  </si>
+  <si>
+    <t>Longest subarray with sum K (Positives + Negatives)</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/longest-subarray-with-sum-k</t>
+  </si>
+  <si>
+    <t>Striver</t>
+  </si>
+  <si>
+    <t>Longest subarray with sum K (Positives Only)</t>
+  </si>
+  <si>
+    <t>Sum, Sliding Window</t>
+  </si>
+  <si>
+    <t>Dutch National Flag</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-colors/submissions/1881574577/</t>
+  </si>
+  <si>
+    <t>3-Pointer</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/majority-element/description/</t>
+  </si>
+  <si>
+    <t>Moore's voting algo</t>
+  </si>
+  <si>
+    <t>PrefixSum+ Hashing</t>
+  </si>
+  <si>
+    <t>Majority element</t>
+  </si>
+  <si>
+    <t>Max Subarray</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-subarray/</t>
+  </si>
+  <si>
+    <t>Kadane's Algo</t>
+  </si>
+  <si>
+    <t>Buy &amp; Sell Stock I</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/submissions/1881708167/</t>
+  </si>
+  <si>
+    <t>Traverse</t>
+  </si>
+  <si>
+    <t>Count Subarray sum equals k</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subarray-sum-equals-k/description/</t>
+  </si>
+  <si>
+    <t>Modified PrefixSum, HashMap</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/spiral-matrix/description/</t>
+  </si>
+  <si>
+    <t>Spiral Matrix</t>
+  </si>
+  <si>
+    <t>Traverse, left-right-top-bottom</t>
   </si>
 </sst>
 </file>
@@ -941,7 +1013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
@@ -3283,16 +3355,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="21.453125" customWidth="1"/>
     <col min="5" max="5" width="14.36328125" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" customWidth="1"/>
     <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3354,9 +3427,238 @@
         <v>46052</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="14">
+        <v>46035</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" s="14">
+        <v>46035</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I5" s="14">
+        <v>46035</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6">
+        <v>169</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" s="14">
+        <v>46035</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I7" s="14">
+        <v>46035</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8">
+        <v>121</v>
+      </c>
+      <c r="D8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="14">
+        <v>46035</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9">
+        <v>560</v>
+      </c>
+      <c r="D9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I9" s="14">
+        <v>46035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I10" s="14">
+        <v>46035</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{446E0945-919F-4C75-A7DF-820B86BF045D}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{6BD9FC8D-D860-4487-813E-05069DABA9B6}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{620BDF33-94AB-4453-9FFD-1A67599134F0}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{1A1F4847-2763-4D4C-B18C-7C66F9415C06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added code for minimum time visiting all points
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA9816A-5FC9-4E77-9CA0-010EFDF52466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FAE628-701C-4923-8491-F7EF63244057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA Tracker" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="182">
   <si>
     <t>ID</t>
   </si>
@@ -572,6 +572,12 @@
   </si>
   <si>
     <t>Traverse, left-right-top-bottom</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subsets/</t>
+  </si>
+  <si>
+    <t>All subsets</t>
   </si>
 </sst>
 </file>
@@ -688,7 +694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -704,7 +710,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1013,21 +1018,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.54296875" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
-    <col min="6" max="6" width="33.1796875" customWidth="1"/>
-    <col min="7" max="7" width="17.54296875" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1076,7 +1081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1098,19 +1103,19 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1129,17 +1134,17 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1158,17 +1163,17 @@
       <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1187,17 +1192,17 @@
       <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1219,17 +1224,17 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1248,17 +1253,17 @@
       <c r="G8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1280,17 +1285,17 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1312,17 +1317,17 @@
       <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1344,17 +1349,17 @@
       <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1373,17 +1378,17 @@
       <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1405,17 +1410,17 @@
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1437,17 +1442,17 @@
       <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1469,17 +1474,17 @@
       <c r="G15" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1501,17 +1506,17 @@
       <c r="G16" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1533,17 +1538,17 @@
       <c r="G17" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1562,17 +1567,17 @@
       <c r="G18" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1594,17 +1599,17 @@
       <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1623,17 +1628,17 @@
       <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1655,17 +1660,17 @@
       <c r="G21" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1687,17 +1692,17 @@
       <c r="G22" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1716,17 +1721,17 @@
       <c r="G23" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1745,17 +1750,17 @@
       <c r="G24" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1774,17 +1779,17 @@
       <c r="G25" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1806,17 +1811,17 @@
       <c r="G26" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1838,17 +1843,17 @@
       <c r="G27" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1870,17 +1875,17 @@
       <c r="G28" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1902,17 +1907,17 @@
       <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1934,17 +1939,17 @@
       <c r="G30" t="s">
         <v>74</v>
       </c>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1963,17 +1968,17 @@
       <c r="G31" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1995,17 +2000,17 @@
       <c r="G32" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2027,17 +2032,17 @@
       <c r="G33" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2059,17 +2064,17 @@
       <c r="G34" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2091,17 +2096,17 @@
       <c r="G35" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2124,7 +2129,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2147,7 +2152,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2170,7 +2175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2193,7 +2198,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2216,7 +2221,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2239,7 +2244,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2268,7 +2273,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2297,7 +2302,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2326,7 +2331,7 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2355,7 +2360,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2381,7 +2386,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2407,7 +2412,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2426,14 +2431,14 @@
       <c r="G48" t="s">
         <v>13</v>
       </c>
-      <c r="H48" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="I48" s="15">
-        <v>46034</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H48" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I48" s="8">
+        <v>46040</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2462,877 +2467,906 @@
         <v>46038</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50">
+        <v>78</v>
+      </c>
+      <c r="D50" t="s">
+        <v>180</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F50" t="s">
+        <v>145</v>
+      </c>
+      <c r="G50" t="s">
+        <v>131</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I50" s="8">
+        <v>46039</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I54" t="str">
         <f>IF(H54="Hard",#REF!+ 3,IF(H54="Medium",#REF!+ 7,IF(H54="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I55" t="str">
         <f>IF(H55="Hard",#REF!+ 3,IF(H55="Medium",#REF!+ 7,IF(H55="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I56" t="str">
         <f>IF(H56="Hard",#REF!+ 3,IF(H56="Medium",#REF!+ 7,IF(H56="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I57" t="str">
         <f>IF(H57="Hard",#REF!+ 3,IF(H57="Medium",#REF!+ 7,IF(H57="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I58" t="str">
         <f>IF(H58="Hard",#REF!+ 3,IF(H58="Medium",#REF!+ 7,IF(H58="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I59" t="str">
         <f>IF(H59="Hard",#REF!+ 3,IF(H59="Medium",#REF!+ 7,IF(H59="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I60" t="str">
         <f>IF(H60="Hard",#REF!+ 3,IF(H60="Medium",#REF!+ 7,IF(H60="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I61" t="str">
         <f>IF(H61="Hard",#REF!+ 3,IF(H61="Medium",#REF!+ 7,IF(H61="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I62" t="str">
         <f>IF(H62="Hard",#REF!+ 3,IF(H62="Medium",#REF!+ 7,IF(H62="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I63" t="str">
         <f>IF(H63="Hard",#REF!+ 3,IF(H63="Medium",#REF!+ 7,IF(H63="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I64" t="str">
         <f>IF(H64="Hard",#REF!+ 3,IF(H64="Medium",#REF!+ 7,IF(H64="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I65" t="str">
         <f>IF(H65="Hard",#REF!+ 3,IF(H65="Medium",#REF!+ 7,IF(H65="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I66" t="str">
         <f>IF(H66="Hard",#REF!+ 3,IF(H66="Medium",#REF!+ 7,IF(H66="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I67" t="str">
         <f>IF(H67="Hard",#REF!+ 3,IF(H67="Medium",#REF!+ 7,IF(H67="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I68" t="str">
         <f>IF(H68="Hard",#REF!+ 3,IF(H68="Medium",#REF!+ 7,IF(H68="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I69" t="str">
         <f>IF(H69="Hard",#REF!+ 3,IF(H69="Medium",#REF!+ 7,IF(H69="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I70" t="str">
         <f>IF(H70="Hard",#REF!+ 3,IF(H70="Medium",#REF!+ 7,IF(H70="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I71" t="str">
         <f>IF(H71="Hard",#REF!+ 3,IF(H71="Medium",#REF!+ 7,IF(H71="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I72" t="str">
         <f>IF(H72="Hard",#REF!+ 3,IF(H72="Medium",#REF!+ 7,IF(H72="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I73" t="str">
         <f>IF(H73="Hard",#REF!+ 3,IF(H73="Medium",#REF!+ 7,IF(H73="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I74" t="str">
         <f>IF(H74="Hard",#REF!+ 3,IF(H74="Medium",#REF!+ 7,IF(H74="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I75" t="str">
         <f>IF(H75="Hard",#REF!+ 3,IF(H75="Medium",#REF!+ 7,IF(H75="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I76" t="str">
         <f>IF(H76="Hard",#REF!+ 3,IF(H76="Medium",#REF!+ 7,IF(H76="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I77" t="str">
         <f>IF(H77="Hard",#REF!+ 3,IF(H77="Medium",#REF!+ 7,IF(H77="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I78" t="str">
         <f>IF(H78="Hard",#REF!+ 3,IF(H78="Medium",#REF!+ 7,IF(H78="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I79" t="str">
         <f>IF(H79="Hard",#REF!+ 3,IF(H79="Medium",#REF!+ 7,IF(H79="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I80" t="str">
         <f>IF(H80="Hard",#REF!+ 3,IF(H80="Medium",#REF!+ 7,IF(H80="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I81" t="str">
         <f>IF(H81="Hard",#REF!+ 3,IF(H81="Medium",#REF!+ 7,IF(H81="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I82" t="str">
         <f>IF(H82="Hard",#REF!+ 3,IF(H82="Medium",#REF!+ 7,IF(H82="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I83" t="str">
         <f>IF(H83="Hard",#REF!+ 3,IF(H83="Medium",#REF!+ 7,IF(H83="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I84" t="str">
         <f>IF(H84="Hard",#REF!+ 3,IF(H84="Medium",#REF!+ 7,IF(H84="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I85" t="str">
         <f>IF(H85="Hard",#REF!+ 3,IF(H85="Medium",#REF!+ 7,IF(H85="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I86" t="str">
         <f>IF(H86="Hard",#REF!+ 3,IF(H86="Medium",#REF!+ 7,IF(H86="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I87" t="str">
         <f>IF(H87="Hard",#REF!+ 3,IF(H87="Medium",#REF!+ 7,IF(H87="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I88" t="str">
         <f>IF(H88="Hard",#REF!+ 3,IF(H88="Medium",#REF!+ 7,IF(H88="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I89" t="str">
         <f>IF(H89="Hard",#REF!+ 3,IF(H89="Medium",#REF!+ 7,IF(H89="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I90" t="str">
         <f>IF(H90="Hard",#REF!+ 3,IF(H90="Medium",#REF!+ 7,IF(H90="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I91" t="str">
         <f>IF(H91="Hard",#REF!+ 3,IF(H91="Medium",#REF!+ 7,IF(H91="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I92" t="str">
         <f>IF(H92="Hard",#REF!+ 3,IF(H92="Medium",#REF!+ 7,IF(H92="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I93" t="str">
         <f>IF(H93="Hard",#REF!+ 3,IF(H93="Medium",#REF!+ 7,IF(H93="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I94" t="str">
         <f>IF(H94="Hard",#REF!+ 3,IF(H94="Medium",#REF!+ 7,IF(H94="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I95" t="str">
         <f>IF(H95="Hard",#REF!+ 3,IF(H95="Medium",#REF!+ 7,IF(H95="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I96" t="str">
         <f>IF(H96="Hard",#REF!+ 3,IF(H96="Medium",#REF!+ 7,IF(H96="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I97" t="str">
         <f>IF(H97="Hard",#REF!+ 3,IF(H97="Medium",#REF!+ 7,IF(H97="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I98" t="str">
         <f>IF(H98="Hard",#REF!+ 3,IF(H98="Medium",#REF!+ 7,IF(H98="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I99" t="str">
         <f>IF(H99="Hard",#REF!+ 3,IF(H99="Medium",#REF!+ 7,IF(H99="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I100" t="str">
         <f>IF(H100="Hard",#REF!+ 3,IF(H100="Medium",#REF!+ 7,IF(H100="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I101" t="str">
         <f>IF(H101="Hard",#REF!+ 3,IF(H101="Medium",#REF!+ 7,IF(H101="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I102" t="str">
         <f>IF(H102="Hard",#REF!+ 3,IF(H102="Medium",#REF!+ 7,IF(H102="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I103" t="str">
         <f>IF(H103="Hard",#REF!+ 3,IF(H103="Medium",#REF!+ 7,IF(H103="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I104" t="str">
         <f>IF(H104="Hard",#REF!+ 3,IF(H104="Medium",#REF!+ 7,IF(H104="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I105" t="str">
         <f>IF(H105="Hard",#REF!+ 3,IF(H105="Medium",#REF!+ 7,IF(H105="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I106" t="str">
         <f>IF(H106="Hard",#REF!+ 3,IF(H106="Medium",#REF!+ 7,IF(H106="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I107" t="str">
         <f>IF(H107="Hard",#REF!+ 3,IF(H107="Medium",#REF!+ 7,IF(H107="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I108" t="str">
         <f>IF(H108="Hard",#REF!+ 3,IF(H108="Medium",#REF!+ 7,IF(H108="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="109" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I109" t="str">
         <f>IF(H109="Hard",#REF!+ 3,IF(H109="Medium",#REF!+ 7,IF(H109="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="110" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I110" t="str">
         <f>IF(H110="Hard",#REF!+ 3,IF(H110="Medium",#REF!+ 7,IF(H110="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="111" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I111" t="str">
         <f>IF(H111="Hard",#REF!+ 3,IF(H111="Medium",#REF!+ 7,IF(H111="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="112" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I112" t="str">
         <f>IF(H112="Hard",#REF!+ 3,IF(H112="Medium",#REF!+ 7,IF(H112="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="113" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I113" t="str">
         <f>IF(H113="Hard",#REF!+ 3,IF(H113="Medium",#REF!+ 7,IF(H113="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="114" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I114" t="str">
         <f>IF(H114="Hard",#REF!+ 3,IF(H114="Medium",#REF!+ 7,IF(H114="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I115" t="str">
         <f>IF(H115="Hard",#REF!+ 3,IF(H115="Medium",#REF!+ 7,IF(H115="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="116" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I116" t="str">
         <f>IF(H116="Hard",#REF!+ 3,IF(H116="Medium",#REF!+ 7,IF(H116="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="117" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I117" t="str">
         <f>IF(H117="Hard",#REF!+ 3,IF(H117="Medium",#REF!+ 7,IF(H117="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="118" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I118" t="str">
         <f>IF(H118="Hard",#REF!+ 3,IF(H118="Medium",#REF!+ 7,IF(H118="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="119" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I119" t="str">
         <f>IF(H119="Hard",#REF!+ 3,IF(H119="Medium",#REF!+ 7,IF(H119="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="120" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I120" t="str">
         <f>IF(H120="Hard",#REF!+ 3,IF(H120="Medium",#REF!+ 7,IF(H120="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="121" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I121" t="str">
         <f>IF(H121="Hard",#REF!+ 3,IF(H121="Medium",#REF!+ 7,IF(H121="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="122" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I122" t="str">
         <f>IF(H122="Hard",#REF!+ 3,IF(H122="Medium",#REF!+ 7,IF(H122="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="123" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I123" t="str">
         <f>IF(H123="Hard",#REF!+ 3,IF(H123="Medium",#REF!+ 7,IF(H123="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="124" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I124" t="str">
         <f>IF(H124="Hard",#REF!+ 3,IF(H124="Medium",#REF!+ 7,IF(H124="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="125" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I125" t="str">
         <f>IF(H125="Hard",#REF!+ 3,IF(H125="Medium",#REF!+ 7,IF(H125="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="126" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I126" t="str">
         <f>IF(H126="Hard",#REF!+ 3,IF(H126="Medium",#REF!+ 7,IF(H126="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="127" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I127" t="str">
         <f>IF(H127="Hard",#REF!+ 3,IF(H127="Medium",#REF!+ 7,IF(H127="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="128" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I128" t="str">
         <f>IF(H128="Hard",#REF!+ 3,IF(H128="Medium",#REF!+ 7,IF(H128="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="129" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I129" t="str">
         <f>IF(H129="Hard",#REF!+ 3,IF(H129="Medium",#REF!+ 7,IF(H129="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="130" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I130" t="str">
         <f>IF(H130="Hard",#REF!+ 3,IF(H130="Medium",#REF!+ 7,IF(H130="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I131" t="str">
         <f>IF(H131="Hard",#REF!+ 3,IF(H131="Medium",#REF!+ 7,IF(H131="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I132" t="str">
         <f>IF(H132="Hard",#REF!+ 3,IF(H132="Medium",#REF!+ 7,IF(H132="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="133" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I133" t="str">
         <f>IF(H133="Hard",#REF!+ 3,IF(H133="Medium",#REF!+ 7,IF(H133="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="134" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I134" t="str">
         <f>IF(H134="Hard",#REF!+ 3,IF(H134="Medium",#REF!+ 7,IF(H134="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="135" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I135" t="str">
         <f>IF(H135="Hard",#REF!+ 3,IF(H135="Medium",#REF!+ 7,IF(H135="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="136" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I136" t="str">
         <f>IF(H136="Hard",#REF!+ 3,IF(H136="Medium",#REF!+ 7,IF(H136="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="137" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I137" t="str">
         <f>IF(H137="Hard",#REF!+ 3,IF(H137="Medium",#REF!+ 7,IF(H137="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="138" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I138" t="str">
         <f>IF(H138="Hard",#REF!+ 3,IF(H138="Medium",#REF!+ 7,IF(H138="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="139" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I139" t="str">
         <f>IF(H139="Hard",#REF!+ 3,IF(H139="Medium",#REF!+ 7,IF(H139="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="140" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I140" t="str">
         <f>IF(H140="Hard",#REF!+ 3,IF(H140="Medium",#REF!+ 7,IF(H140="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="141" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I141" t="str">
         <f>IF(H141="Hard",#REF!+ 3,IF(H141="Medium",#REF!+ 7,IF(H141="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="142" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I142" t="str">
         <f>IF(H142="Hard",#REF!+ 3,IF(H142="Medium",#REF!+ 7,IF(H142="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="143" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I143" t="str">
         <f>IF(H143="Hard",#REF!+ 3,IF(H143="Medium",#REF!+ 7,IF(H143="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="144" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I144" t="str">
         <f>IF(H144="Hard",#REF!+ 3,IF(H144="Medium",#REF!+ 7,IF(H144="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="145" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I145" t="str">
         <f>IF(H145="Hard",#REF!+ 3,IF(H145="Medium",#REF!+ 7,IF(H145="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="146" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I146" t="str">
         <f>IF(H146="Hard",#REF!+ 3,IF(H146="Medium",#REF!+ 7,IF(H146="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="147" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I147" t="str">
         <f>IF(H147="Hard",#REF!+ 3,IF(H147="Medium",#REF!+ 7,IF(H147="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="148" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I148" t="str">
         <f>IF(H148="Hard",#REF!+ 3,IF(H148="Medium",#REF!+ 7,IF(H148="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="149" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I149" t="str">
         <f>IF(H149="Hard",#REF!+ 3,IF(H149="Medium",#REF!+ 7,IF(H149="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="150" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I150" t="str">
         <f>IF(H150="Hard",#REF!+ 3,IF(H150="Medium",#REF!+ 7,IF(H150="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="151" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I151" t="str">
         <f>IF(H151="Hard",#REF!+ 3,IF(H151="Medium",#REF!+ 7,IF(H151="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="152" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I152" t="str">
         <f>IF(H152="Hard",#REF!+ 3,IF(H152="Medium",#REF!+ 7,IF(H152="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="153" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I153" t="str">
         <f>IF(H153="Hard",#REF!+ 3,IF(H153="Medium",#REF!+ 7,IF(H153="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="154" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I154" t="str">
         <f>IF(H154="Hard",#REF!+ 3,IF(H154="Medium",#REF!+ 7,IF(H154="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="155" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I155" t="str">
         <f>IF(H155="Hard",#REF!+ 3,IF(H155="Medium",#REF!+ 7,IF(H155="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="156" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I156" t="str">
         <f>IF(H156="Hard",#REF!+ 3,IF(H156="Medium",#REF!+ 7,IF(H156="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="157" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I157" t="str">
         <f>IF(H157="Hard",#REF!+ 3,IF(H157="Medium",#REF!+ 7,IF(H157="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="158" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I158" t="str">
         <f>IF(H158="Hard",#REF!+ 3,IF(H158="Medium",#REF!+ 7,IF(H158="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="159" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I159" t="str">
         <f>IF(H159="Hard",#REF!+ 3,IF(H159="Medium",#REF!+ 7,IF(H159="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="160" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I160" t="str">
         <f>IF(H160="Hard",#REF!+ 3,IF(H160="Medium",#REF!+ 7,IF(H160="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="161" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I161" t="str">
         <f>IF(H161="Hard",#REF!+ 3,IF(H161="Medium",#REF!+ 7,IF(H161="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="162" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="162" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I162" t="str">
         <f>IF(H162="Hard",#REF!+ 3,IF(H162="Medium",#REF!+ 7,IF(H162="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="163" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="163" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I163" t="str">
         <f>IF(H163="Hard",#REF!+ 3,IF(H163="Medium",#REF!+ 7,IF(H163="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="164" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="164" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I164" t="str">
         <f>IF(H164="Hard",#REF!+ 3,IF(H164="Medium",#REF!+ 7,IF(H164="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="165" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="165" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I165" t="str">
         <f>IF(H165="Hard",#REF!+ 3,IF(H165="Medium",#REF!+ 7,IF(H165="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="166" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="166" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I166" t="str">
         <f>IF(H166="Hard",#REF!+ 3,IF(H166="Medium",#REF!+ 7,IF(H166="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="167" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I167" t="str">
         <f>IF(H167="Hard",#REF!+ 3,IF(H167="Medium",#REF!+ 7,IF(H167="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="168" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="168" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I168" t="str">
         <f>IF(H168="Hard",#REF!+ 3,IF(H168="Medium",#REF!+ 7,IF(H168="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="169" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I169" t="str">
         <f>IF(H169="Hard",#REF!+ 3,IF(H169="Medium",#REF!+ 7,IF(H169="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="170" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="170" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I170" t="str">
         <f>IF(H170="Hard",#REF!+ 3,IF(H170="Medium",#REF!+ 7,IF(H170="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="171" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="171" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I171" t="str">
         <f>IF(H171="Hard",#REF!+ 3,IF(H171="Medium",#REF!+ 7,IF(H171="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="172" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="172" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I172" t="str">
         <f>IF(H172="Hard",#REF!+ 3,IF(H172="Medium",#REF!+ 7,IF(H172="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="173" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="173" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I173" t="str">
         <f>IF(H173="Hard",#REF!+ 3,IF(H173="Medium",#REF!+ 7,IF(H173="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="174" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="174" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I174" t="str">
         <f>IF(H174="Hard",#REF!+ 3,IF(H174="Medium",#REF!+ 7,IF(H174="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="175" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="175" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I175" t="str">
         <f>IF(H175="Hard",#REF!+ 3,IF(H175="Medium",#REF!+ 7,IF(H175="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="176" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="176" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I176" t="str">
         <f>IF(H176="Hard",#REF!+ 3,IF(H176="Medium",#REF!+ 7,IF(H176="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="177" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I177" t="str">
         <f>IF(H177="Hard",#REF!+ 3,IF(H177="Medium",#REF!+ 7,IF(H177="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="178" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I178" t="str">
         <f>IF(H178="Hard",#REF!+ 3,IF(H178="Medium",#REF!+ 7,IF(H178="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="179" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I179" t="str">
         <f>IF(H179="Hard",#REF!+ 3,IF(H179="Medium",#REF!+ 7,IF(H179="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="180" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I180" t="str">
         <f>IF(H180="Hard",#REF!+ 3,IF(H180="Medium",#REF!+ 7,IF(H180="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="181" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="181" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I181" t="str">
         <f>IF(H181="Hard",#REF!+ 3,IF(H181="Medium",#REF!+ 7,IF(H181="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="182" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I182" t="str">
         <f>IF(H182="Hard",#REF!+ 3,IF(H182="Medium",#REF!+ 7,IF(H182="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="183" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="183" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I183" t="str">
         <f>IF(H183="Hard",#REF!+ 3,IF(H183="Medium",#REF!+ 7,IF(H183="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="184" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I184" t="str">
         <f>IF(H184="Hard",#REF!+ 3,IF(H184="Medium",#REF!+ 7,IF(H184="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I185" t="str">
         <f>IF(H185="Hard",#REF!+ 3,IF(H185="Medium",#REF!+ 7,IF(H185="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="186" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I186" t="str">
         <f>IF(H186="Hard",#REF!+ 3,IF(H186="Medium",#REF!+ 7,IF(H186="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="187" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="187" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I187" t="str">
         <f>IF(H187="Hard",#REF!+ 3,IF(H187="Medium",#REF!+ 7,IF(H187="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="188" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I188" t="str">
         <f>IF(H188="Hard",#REF!+ 3,IF(H188="Medium",#REF!+ 7,IF(H188="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="189" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I189" t="str">
         <f>IF(H189="Hard",#REF!+ 3,IF(H189="Medium",#REF!+ 7,IF(H189="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="190" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I190" t="str">
         <f>IF(H190="Hard",#REF!+ 3,IF(H190="Medium",#REF!+ 7,IF(H190="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="191" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="191" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I191" t="str">
         <f>IF(H191="Hard",#REF!+ 3,IF(H191="Medium",#REF!+ 7,IF(H191="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="192" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="192" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I192" t="str">
         <f>IF(H192="Hard",#REF!+ 3,IF(H192="Medium",#REF!+ 7,IF(H192="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="193" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I193" t="str">
         <f>IF(H193="Hard",#REF!+ 3,IF(H193="Medium",#REF!+ 7,IF(H193="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="194" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="194" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I194" t="str">
         <f>IF(H194="Hard",#REF!+ 3,IF(H194="Medium",#REF!+ 7,IF(H194="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="195" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="195" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I195" t="str">
         <f>IF(H195="Hard",#REF!+ 3,IF(H195="Medium",#REF!+ 7,IF(H195="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="196" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I196" t="str">
         <f>IF(H196="Hard",#REF!+ 3,IF(H196="Medium",#REF!+ 7,IF(H196="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="197" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="197" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I197" t="str">
         <f>IF(H197="Hard",#REF!+ 3,IF(H197="Medium",#REF!+ 7,IF(H197="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="198" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="198" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I198" t="str">
         <f>IF(H198="Hard",#REF!+ 3,IF(H198="Medium",#REF!+ 7,IF(H198="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="199" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="199" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I199" t="str">
         <f>IF(H199="Hard",#REF!+ 3,IF(H199="Medium",#REF!+ 7,IF(H199="Easy",#REF!+ 30,"")))</f>
         <v/>
@@ -3357,19 +3391,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" customWidth="1"/>
-    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3398,7 +3432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3427,7 +3461,7 @@
         <v>46052</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3453,7 +3487,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3479,7 +3513,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3508,7 +3542,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3537,7 +3571,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3566,7 +3600,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3595,7 +3629,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3624,7 +3658,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Added code for daily challenge day 13
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FAE628-701C-4923-8491-F7EF63244057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF51B998-AD4F-4BCC-951C-1A8A4E5AF56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="190">
   <si>
     <t>ID</t>
   </si>
@@ -578,6 +578,30 @@
   </si>
   <si>
     <t>All subsets</t>
+  </si>
+  <si>
+    <t>Next Permutation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/next-permutation/</t>
+  </si>
+  <si>
+    <t>Traverse, Reverse</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-consecutive-sequence/</t>
+  </si>
+  <si>
+    <t>Traverse, Hashing</t>
+  </si>
+  <si>
+    <t>Pascal's triangle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/pascals-triangle/description/</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="O59" sqref="O59"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,6 +1104,12 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
+      <c r="H2" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2" s="14">
+        <v>46065</v>
+      </c>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1102,6 +1132,12 @@
       </c>
       <c r="G3" t="s">
         <v>17</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" s="14">
+        <v>46065</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>127</v>
@@ -1133,6 +1169,12 @@
       </c>
       <c r="G4" t="s">
         <v>13</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I4" s="14">
+        <v>46065</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
@@ -1163,6 +1205,12 @@
       <c r="G5" t="s">
         <v>13</v>
       </c>
+      <c r="H5" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="14">
+        <v>46065</v>
+      </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
@@ -1192,6 +1240,12 @@
       <c r="G6" t="s">
         <v>13</v>
       </c>
+      <c r="H6" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I6" s="14">
+        <v>46065</v>
+      </c>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
@@ -1224,6 +1278,12 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
+      <c r="H7" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I7" s="14">
+        <v>46065</v>
+      </c>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
@@ -1253,6 +1313,12 @@
       <c r="G8" t="s">
         <v>13</v>
       </c>
+      <c r="H8" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="14">
+        <v>46040</v>
+      </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
@@ -1285,6 +1351,12 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
+      <c r="H9" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I9" s="14">
+        <v>46036</v>
+      </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
@@ -1317,6 +1389,12 @@
       <c r="G10" t="s">
         <v>17</v>
       </c>
+      <c r="H10" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I10" s="14">
+        <v>46065</v>
+      </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
@@ -1349,6 +1427,12 @@
       <c r="G11" t="s">
         <v>17</v>
       </c>
+      <c r="H11" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I11" s="14">
+        <v>46065</v>
+      </c>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
@@ -1378,6 +1462,12 @@
       <c r="G12" t="s">
         <v>13</v>
       </c>
+      <c r="H12" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I12" s="14">
+        <v>46065</v>
+      </c>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
@@ -1410,6 +1500,12 @@
       <c r="G13" t="s">
         <v>17</v>
       </c>
+      <c r="H13" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I13" s="14">
+        <v>46065</v>
+      </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
@@ -2383,7 +2479,7 @@
         <v>139</v>
       </c>
       <c r="I46" s="8">
-        <v>46035</v>
+        <v>46037</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -3389,10 +3485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3400,7 +3496,7 @@
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3480,11 +3576,11 @@
       <c r="G3" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>139</v>
+      <c r="H3" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="I3" s="14">
-        <v>46035</v>
+        <v>46041</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3506,11 +3602,11 @@
       <c r="G4" t="s">
         <v>158</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>139</v>
+      <c r="H4" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="I4" s="14">
-        <v>46035</v>
+        <v>46041</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3523,7 +3619,7 @@
       <c r="C5">
         <v>75</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="10" t="s">
         <v>162</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -3535,11 +3631,11 @@
       <c r="G5" t="s">
         <v>131</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>139</v>
+      <c r="H5" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="I5" s="14">
-        <v>46035</v>
+        <v>46041</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3564,11 +3660,11 @@
       <c r="G6" t="s">
         <v>131</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>139</v>
+      <c r="H6" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="I6" s="14">
-        <v>46035</v>
+        <v>46041</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3581,7 +3677,7 @@
       <c r="C7">
         <v>53</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="10" t="s">
         <v>169</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -3597,7 +3693,7 @@
         <v>139</v>
       </c>
       <c r="I7" s="14">
-        <v>46035</v>
+        <v>46037</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3622,11 +3718,11 @@
       <c r="G8" t="s">
         <v>131</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>139</v>
+      <c r="H8" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="I8" s="14">
-        <v>46035</v>
+        <v>46041</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3651,11 +3747,11 @@
       <c r="G9" t="s">
         <v>131</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>139</v>
+      <c r="H9" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="I9" s="14">
-        <v>46035</v>
+        <v>46041</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3680,11 +3776,98 @@
       <c r="G10" t="s">
         <v>131</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" s="14">
+        <v>46041</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
+        <v>184</v>
+      </c>
+      <c r="G11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="I10" s="14">
-        <v>46035</v>
+      <c r="I11" s="14">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12">
+        <v>128</v>
+      </c>
+      <c r="D12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G12" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="14">
+        <v>46040</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13">
+        <v>118</v>
+      </c>
+      <c r="D13" t="s">
+        <v>189</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>173</v>
+      </c>
+      <c r="G13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I13" s="14">
+        <v>46040</v>
       </c>
     </row>
   </sheetData>
@@ -3693,6 +3876,8 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{6BD9FC8D-D860-4487-813E-05069DABA9B6}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{620BDF33-94AB-4453-9FFD-1A67599134F0}"/>
     <hyperlink ref="D6" r:id="rId4" xr:uid="{1A1F4847-2763-4D4C-B18C-7C66F9415C06}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{5D75CC5B-790A-4135-9505-78843D9EC616}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{47EE779C-1BE0-4B40-9A27-5425F3C420B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added updated excel sheet
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF51B998-AD4F-4BCC-951C-1A8A4E5AF56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87016EE6-55B6-4D6D-B7DA-756954558137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA Tracker" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="219">
   <si>
     <t>ID</t>
   </si>
@@ -415,9 +415,6 @@
     <t>Implementation</t>
   </si>
   <si>
-    <t>From Monday Revision+ company-wise practice</t>
-  </si>
-  <si>
     <t>Max product of sum of subtrees</t>
   </si>
   <si>
@@ -602,6 +599,96 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/pascals-triangle/description/</t>
+  </si>
+  <si>
+    <t>From Monday Revision</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/majority-element-ii/description/</t>
+  </si>
+  <si>
+    <t>Moore's Voting algo, traverse</t>
+  </si>
+  <si>
+    <t>3 sum</t>
+  </si>
+  <si>
+    <t>Majority Element 2</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/3sum/description/</t>
+  </si>
+  <si>
+    <t>Traversal + 2 Pointer</t>
+  </si>
+  <si>
+    <t>4 Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/4sum/description/</t>
+  </si>
+  <si>
+    <t>Largest subarray with sum 0</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/largest-subarray-with-sum-0</t>
+  </si>
+  <si>
+    <t>prefixSum + Hashing</t>
+  </si>
+  <si>
+    <t>Count subarrays with xor k</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/count-subarrays-with-given-xor-k</t>
+  </si>
+  <si>
+    <t>prefixXOR + Hashing</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-intervals/</t>
+  </si>
+  <si>
+    <t>Merge intervals</t>
+  </si>
+  <si>
+    <t>Merge arrays</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-sorted-array/description/</t>
+  </si>
+  <si>
+    <t>Find missing &amp; repeating number</t>
+  </si>
+  <si>
+    <t>Maths, Formulas</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/find-the-repeating-and-missing-number</t>
+  </si>
+  <si>
+    <t>Count Inversions</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/count-inversions</t>
+  </si>
+  <si>
+    <t>Pure merge Sort with count frequency count</t>
+  </si>
+  <si>
+    <t>Reverse Pairs</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-pairs/</t>
+  </si>
+  <si>
+    <t>Merge Sort</t>
+  </si>
+  <si>
+    <t>Max Product subarray</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-product-subarray/description/</t>
   </si>
 </sst>
 </file>
@@ -1042,21 +1129,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView topLeftCell="A34" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" customWidth="1"/>
+    <col min="6" max="6" width="33.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1105,13 +1192,13 @@
         <v>13</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I2" s="14">
         <v>46065</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1134,13 +1221,13 @@
         <v>17</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I3" s="14">
         <v>46065</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>127</v>
+        <v>189</v>
       </c>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
@@ -1151,7 +1238,7 @@
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1171,7 +1258,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I4" s="14">
         <v>46065</v>
@@ -1186,7 +1273,7 @@
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1206,7 +1293,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I5" s="14">
         <v>46065</v>
@@ -1221,7 +1308,7 @@
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1241,7 +1328,7 @@
         <v>13</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I6" s="14">
         <v>46065</v>
@@ -1256,7 +1343,7 @@
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1279,7 +1366,7 @@
         <v>17</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I7" s="14">
         <v>46065</v>
@@ -1294,7 +1381,7 @@
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1314,7 +1401,7 @@
         <v>13</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I8" s="14">
         <v>46040</v>
@@ -1329,7 +1416,7 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1352,7 +1439,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I9" s="14">
         <v>46036</v>
@@ -1367,7 +1454,7 @@
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1390,7 +1477,7 @@
         <v>17</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I10" s="14">
         <v>46065</v>
@@ -1405,7 +1492,7 @@
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1428,7 +1515,7 @@
         <v>17</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I11" s="14">
         <v>46065</v>
@@ -1443,7 +1530,7 @@
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1463,7 +1550,7 @@
         <v>13</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I12" s="14">
         <v>46065</v>
@@ -1478,7 +1565,7 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1501,7 +1588,7 @@
         <v>17</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I13" s="14">
         <v>46065</v>
@@ -1516,7 +1603,7 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1537,6 +1624,12 @@
       </c>
       <c r="G14" t="s">
         <v>17</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" s="14">
+        <v>46041</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
@@ -1548,7 +1641,7 @@
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1569,6 +1662,12 @@
       </c>
       <c r="G15" t="s">
         <v>17</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I15" s="14">
+        <v>46066</v>
       </c>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
@@ -1580,7 +1679,7 @@
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1601,6 +1700,12 @@
       </c>
       <c r="G16" t="s">
         <v>17</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I16" s="14">
+        <v>46066</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
@@ -1612,7 +1717,7 @@
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1633,6 +1738,12 @@
       </c>
       <c r="G17" t="s">
         <v>17</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I17" s="14">
+        <v>46066</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
@@ -1644,7 +1755,7 @@
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1673,7 +1784,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1705,7 +1816,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1734,7 +1845,7 @@
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1766,7 +1877,7 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1798,7 +1909,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1827,7 +1938,7 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1856,7 +1967,7 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1885,7 +1996,7 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1917,7 +2028,7 @@
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1949,7 +2060,7 @@
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1981,7 +2092,7 @@
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2013,7 +2124,7 @@
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2045,7 +2156,7 @@
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2074,7 +2185,7 @@
       <c r="Q31" s="15"/>
       <c r="R31" s="15"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2106,7 +2217,7 @@
       <c r="Q32" s="15"/>
       <c r="R32" s="15"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2138,7 +2249,7 @@
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2170,7 +2281,7 @@
       <c r="Q34" s="15"/>
       <c r="R34" s="15"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2202,7 +2313,7 @@
       <c r="Q35" s="15"/>
       <c r="R35" s="15"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2225,7 +2336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2248,7 +2359,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2271,7 +2382,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2294,7 +2405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2317,7 +2428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2340,1129 +2451,1129 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C42">
         <v>1339</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>119</v>
       </c>
       <c r="F42" t="s">
+        <v>129</v>
+      </c>
+      <c r="G42" t="s">
         <v>130</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I42" s="8">
         <v>46035</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C43">
         <v>50</v>
       </c>
       <c r="D43" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="F43" t="s">
         <v>135</v>
       </c>
-      <c r="F43" t="s">
-        <v>136</v>
-      </c>
       <c r="G43" t="s">
+        <v>130</v>
+      </c>
+      <c r="H43" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I43" s="8">
         <v>46037</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44">
         <v>8</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G44" t="s">
+        <v>130</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I44" s="8">
         <v>46039</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C45">
         <v>1922</v>
       </c>
       <c r="D45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E45" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" t="s">
         <v>135</v>
-      </c>
-      <c r="F45" t="s">
-        <v>136</v>
       </c>
       <c r="G45" t="s">
         <v>17</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I45" s="8">
         <v>46037</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F46" t="s">
         <v>144</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F46" t="s">
-        <v>145</v>
       </c>
       <c r="G46" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I46" s="8">
         <v>46037</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>145</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>147</v>
-      </c>
       <c r="E47" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G47" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I47" s="8">
         <v>46037</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G48" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I48" s="8">
         <v>46040</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C49">
         <v>22</v>
       </c>
       <c r="D49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G49" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I49" s="8">
         <v>46038</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C50">
         <v>78</v>
       </c>
       <c r="D50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G50" t="s">
+        <v>130</v>
+      </c>
+      <c r="H50" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H50" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I50" s="8">
         <v>46039</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I54" t="str">
         <f>IF(H54="Hard",#REF!+ 3,IF(H54="Medium",#REF!+ 7,IF(H54="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I55" t="str">
         <f>IF(H55="Hard",#REF!+ 3,IF(H55="Medium",#REF!+ 7,IF(H55="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I56" t="str">
         <f>IF(H56="Hard",#REF!+ 3,IF(H56="Medium",#REF!+ 7,IF(H56="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I57" t="str">
         <f>IF(H57="Hard",#REF!+ 3,IF(H57="Medium",#REF!+ 7,IF(H57="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I58" t="str">
         <f>IF(H58="Hard",#REF!+ 3,IF(H58="Medium",#REF!+ 7,IF(H58="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I59" t="str">
         <f>IF(H59="Hard",#REF!+ 3,IF(H59="Medium",#REF!+ 7,IF(H59="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I60" t="str">
         <f>IF(H60="Hard",#REF!+ 3,IF(H60="Medium",#REF!+ 7,IF(H60="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I61" t="str">
         <f>IF(H61="Hard",#REF!+ 3,IF(H61="Medium",#REF!+ 7,IF(H61="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I62" t="str">
         <f>IF(H62="Hard",#REF!+ 3,IF(H62="Medium",#REF!+ 7,IF(H62="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I63" t="str">
         <f>IF(H63="Hard",#REF!+ 3,IF(H63="Medium",#REF!+ 7,IF(H63="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I64" t="str">
         <f>IF(H64="Hard",#REF!+ 3,IF(H64="Medium",#REF!+ 7,IF(H64="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I65" t="str">
         <f>IF(H65="Hard",#REF!+ 3,IF(H65="Medium",#REF!+ 7,IF(H65="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I66" t="str">
         <f>IF(H66="Hard",#REF!+ 3,IF(H66="Medium",#REF!+ 7,IF(H66="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I67" t="str">
         <f>IF(H67="Hard",#REF!+ 3,IF(H67="Medium",#REF!+ 7,IF(H67="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I68" t="str">
         <f>IF(H68="Hard",#REF!+ 3,IF(H68="Medium",#REF!+ 7,IF(H68="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I69" t="str">
         <f>IF(H69="Hard",#REF!+ 3,IF(H69="Medium",#REF!+ 7,IF(H69="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I70" t="str">
         <f>IF(H70="Hard",#REF!+ 3,IF(H70="Medium",#REF!+ 7,IF(H70="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I71" t="str">
         <f>IF(H71="Hard",#REF!+ 3,IF(H71="Medium",#REF!+ 7,IF(H71="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I72" t="str">
         <f>IF(H72="Hard",#REF!+ 3,IF(H72="Medium",#REF!+ 7,IF(H72="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I73" t="str">
         <f>IF(H73="Hard",#REF!+ 3,IF(H73="Medium",#REF!+ 7,IF(H73="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I74" t="str">
         <f>IF(H74="Hard",#REF!+ 3,IF(H74="Medium",#REF!+ 7,IF(H74="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I75" t="str">
         <f>IF(H75="Hard",#REF!+ 3,IF(H75="Medium",#REF!+ 7,IF(H75="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I76" t="str">
         <f>IF(H76="Hard",#REF!+ 3,IF(H76="Medium",#REF!+ 7,IF(H76="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I77" t="str">
         <f>IF(H77="Hard",#REF!+ 3,IF(H77="Medium",#REF!+ 7,IF(H77="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I78" t="str">
         <f>IF(H78="Hard",#REF!+ 3,IF(H78="Medium",#REF!+ 7,IF(H78="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I79" t="str">
         <f>IF(H79="Hard",#REF!+ 3,IF(H79="Medium",#REF!+ 7,IF(H79="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I80" t="str">
         <f>IF(H80="Hard",#REF!+ 3,IF(H80="Medium",#REF!+ 7,IF(H80="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I81" t="str">
         <f>IF(H81="Hard",#REF!+ 3,IF(H81="Medium",#REF!+ 7,IF(H81="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I82" t="str">
         <f>IF(H82="Hard",#REF!+ 3,IF(H82="Medium",#REF!+ 7,IF(H82="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I83" t="str">
         <f>IF(H83="Hard",#REF!+ 3,IF(H83="Medium",#REF!+ 7,IF(H83="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I84" t="str">
         <f>IF(H84="Hard",#REF!+ 3,IF(H84="Medium",#REF!+ 7,IF(H84="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I85" t="str">
         <f>IF(H85="Hard",#REF!+ 3,IF(H85="Medium",#REF!+ 7,IF(H85="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I86" t="str">
         <f>IF(H86="Hard",#REF!+ 3,IF(H86="Medium",#REF!+ 7,IF(H86="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I87" t="str">
         <f>IF(H87="Hard",#REF!+ 3,IF(H87="Medium",#REF!+ 7,IF(H87="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I88" t="str">
         <f>IF(H88="Hard",#REF!+ 3,IF(H88="Medium",#REF!+ 7,IF(H88="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I89" t="str">
         <f>IF(H89="Hard",#REF!+ 3,IF(H89="Medium",#REF!+ 7,IF(H89="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I90" t="str">
         <f>IF(H90="Hard",#REF!+ 3,IF(H90="Medium",#REF!+ 7,IF(H90="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I91" t="str">
         <f>IF(H91="Hard",#REF!+ 3,IF(H91="Medium",#REF!+ 7,IF(H91="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I92" t="str">
         <f>IF(H92="Hard",#REF!+ 3,IF(H92="Medium",#REF!+ 7,IF(H92="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I93" t="str">
         <f>IF(H93="Hard",#REF!+ 3,IF(H93="Medium",#REF!+ 7,IF(H93="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I94" t="str">
         <f>IF(H94="Hard",#REF!+ 3,IF(H94="Medium",#REF!+ 7,IF(H94="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I95" t="str">
         <f>IF(H95="Hard",#REF!+ 3,IF(H95="Medium",#REF!+ 7,IF(H95="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I96" t="str">
         <f>IF(H96="Hard",#REF!+ 3,IF(H96="Medium",#REF!+ 7,IF(H96="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I97" t="str">
         <f>IF(H97="Hard",#REF!+ 3,IF(H97="Medium",#REF!+ 7,IF(H97="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I98" t="str">
         <f>IF(H98="Hard",#REF!+ 3,IF(H98="Medium",#REF!+ 7,IF(H98="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I99" t="str">
         <f>IF(H99="Hard",#REF!+ 3,IF(H99="Medium",#REF!+ 7,IF(H99="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I100" t="str">
         <f>IF(H100="Hard",#REF!+ 3,IF(H100="Medium",#REF!+ 7,IF(H100="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I101" t="str">
         <f>IF(H101="Hard",#REF!+ 3,IF(H101="Medium",#REF!+ 7,IF(H101="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I102" t="str">
         <f>IF(H102="Hard",#REF!+ 3,IF(H102="Medium",#REF!+ 7,IF(H102="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I103" t="str">
         <f>IF(H103="Hard",#REF!+ 3,IF(H103="Medium",#REF!+ 7,IF(H103="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I104" t="str">
         <f>IF(H104="Hard",#REF!+ 3,IF(H104="Medium",#REF!+ 7,IF(H104="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I105" t="str">
         <f>IF(H105="Hard",#REF!+ 3,IF(H105="Medium",#REF!+ 7,IF(H105="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I106" t="str">
         <f>IF(H106="Hard",#REF!+ 3,IF(H106="Medium",#REF!+ 7,IF(H106="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I107" t="str">
         <f>IF(H107="Hard",#REF!+ 3,IF(H107="Medium",#REF!+ 7,IF(H107="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I108" t="str">
         <f>IF(H108="Hard",#REF!+ 3,IF(H108="Medium",#REF!+ 7,IF(H108="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I109" t="str">
         <f>IF(H109="Hard",#REF!+ 3,IF(H109="Medium",#REF!+ 7,IF(H109="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I110" t="str">
         <f>IF(H110="Hard",#REF!+ 3,IF(H110="Medium",#REF!+ 7,IF(H110="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I111" t="str">
         <f>IF(H111="Hard",#REF!+ 3,IF(H111="Medium",#REF!+ 7,IF(H111="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I112" t="str">
         <f>IF(H112="Hard",#REF!+ 3,IF(H112="Medium",#REF!+ 7,IF(H112="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I113" t="str">
         <f>IF(H113="Hard",#REF!+ 3,IF(H113="Medium",#REF!+ 7,IF(H113="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="114" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I114" t="str">
         <f>IF(H114="Hard",#REF!+ 3,IF(H114="Medium",#REF!+ 7,IF(H114="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I115" t="str">
         <f>IF(H115="Hard",#REF!+ 3,IF(H115="Medium",#REF!+ 7,IF(H115="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="116" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I116" t="str">
         <f>IF(H116="Hard",#REF!+ 3,IF(H116="Medium",#REF!+ 7,IF(H116="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="117" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I117" t="str">
         <f>IF(H117="Hard",#REF!+ 3,IF(H117="Medium",#REF!+ 7,IF(H117="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I118" t="str">
         <f>IF(H118="Hard",#REF!+ 3,IF(H118="Medium",#REF!+ 7,IF(H118="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="119" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I119" t="str">
         <f>IF(H119="Hard",#REF!+ 3,IF(H119="Medium",#REF!+ 7,IF(H119="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="120" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I120" t="str">
         <f>IF(H120="Hard",#REF!+ 3,IF(H120="Medium",#REF!+ 7,IF(H120="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="121" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I121" t="str">
         <f>IF(H121="Hard",#REF!+ 3,IF(H121="Medium",#REF!+ 7,IF(H121="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="122" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I122" t="str">
         <f>IF(H122="Hard",#REF!+ 3,IF(H122="Medium",#REF!+ 7,IF(H122="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="123" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I123" t="str">
         <f>IF(H123="Hard",#REF!+ 3,IF(H123="Medium",#REF!+ 7,IF(H123="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="124" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I124" t="str">
         <f>IF(H124="Hard",#REF!+ 3,IF(H124="Medium",#REF!+ 7,IF(H124="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="125" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I125" t="str">
         <f>IF(H125="Hard",#REF!+ 3,IF(H125="Medium",#REF!+ 7,IF(H125="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="126" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I126" t="str">
         <f>IF(H126="Hard",#REF!+ 3,IF(H126="Medium",#REF!+ 7,IF(H126="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="127" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I127" t="str">
         <f>IF(H127="Hard",#REF!+ 3,IF(H127="Medium",#REF!+ 7,IF(H127="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="128" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I128" t="str">
         <f>IF(H128="Hard",#REF!+ 3,IF(H128="Medium",#REF!+ 7,IF(H128="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="129" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I129" t="str">
         <f>IF(H129="Hard",#REF!+ 3,IF(H129="Medium",#REF!+ 7,IF(H129="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="130" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I130" t="str">
         <f>IF(H130="Hard",#REF!+ 3,IF(H130="Medium",#REF!+ 7,IF(H130="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I131" t="str">
         <f>IF(H131="Hard",#REF!+ 3,IF(H131="Medium",#REF!+ 7,IF(H131="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I132" t="str">
         <f>IF(H132="Hard",#REF!+ 3,IF(H132="Medium",#REF!+ 7,IF(H132="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="133" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I133" t="str">
         <f>IF(H133="Hard",#REF!+ 3,IF(H133="Medium",#REF!+ 7,IF(H133="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="134" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I134" t="str">
         <f>IF(H134="Hard",#REF!+ 3,IF(H134="Medium",#REF!+ 7,IF(H134="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="135" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I135" t="str">
         <f>IF(H135="Hard",#REF!+ 3,IF(H135="Medium",#REF!+ 7,IF(H135="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="136" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I136" t="str">
         <f>IF(H136="Hard",#REF!+ 3,IF(H136="Medium",#REF!+ 7,IF(H136="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="137" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I137" t="str">
         <f>IF(H137="Hard",#REF!+ 3,IF(H137="Medium",#REF!+ 7,IF(H137="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="138" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I138" t="str">
         <f>IF(H138="Hard",#REF!+ 3,IF(H138="Medium",#REF!+ 7,IF(H138="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="139" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I139" t="str">
         <f>IF(H139="Hard",#REF!+ 3,IF(H139="Medium",#REF!+ 7,IF(H139="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="140" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I140" t="str">
         <f>IF(H140="Hard",#REF!+ 3,IF(H140="Medium",#REF!+ 7,IF(H140="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="141" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I141" t="str">
         <f>IF(H141="Hard",#REF!+ 3,IF(H141="Medium",#REF!+ 7,IF(H141="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="142" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I142" t="str">
         <f>IF(H142="Hard",#REF!+ 3,IF(H142="Medium",#REF!+ 7,IF(H142="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="143" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I143" t="str">
         <f>IF(H143="Hard",#REF!+ 3,IF(H143="Medium",#REF!+ 7,IF(H143="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="144" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I144" t="str">
         <f>IF(H144="Hard",#REF!+ 3,IF(H144="Medium",#REF!+ 7,IF(H144="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="145" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I145" t="str">
         <f>IF(H145="Hard",#REF!+ 3,IF(H145="Medium",#REF!+ 7,IF(H145="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="146" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I146" t="str">
         <f>IF(H146="Hard",#REF!+ 3,IF(H146="Medium",#REF!+ 7,IF(H146="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="147" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I147" t="str">
         <f>IF(H147="Hard",#REF!+ 3,IF(H147="Medium",#REF!+ 7,IF(H147="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="148" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I148" t="str">
         <f>IF(H148="Hard",#REF!+ 3,IF(H148="Medium",#REF!+ 7,IF(H148="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="149" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I149" t="str">
         <f>IF(H149="Hard",#REF!+ 3,IF(H149="Medium",#REF!+ 7,IF(H149="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="150" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I150" t="str">
         <f>IF(H150="Hard",#REF!+ 3,IF(H150="Medium",#REF!+ 7,IF(H150="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="151" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I151" t="str">
         <f>IF(H151="Hard",#REF!+ 3,IF(H151="Medium",#REF!+ 7,IF(H151="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="152" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I152" t="str">
         <f>IF(H152="Hard",#REF!+ 3,IF(H152="Medium",#REF!+ 7,IF(H152="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="153" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I153" t="str">
         <f>IF(H153="Hard",#REF!+ 3,IF(H153="Medium",#REF!+ 7,IF(H153="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="154" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I154" t="str">
         <f>IF(H154="Hard",#REF!+ 3,IF(H154="Medium",#REF!+ 7,IF(H154="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="155" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I155" t="str">
         <f>IF(H155="Hard",#REF!+ 3,IF(H155="Medium",#REF!+ 7,IF(H155="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="156" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I156" t="str">
         <f>IF(H156="Hard",#REF!+ 3,IF(H156="Medium",#REF!+ 7,IF(H156="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="157" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I157" t="str">
         <f>IF(H157="Hard",#REF!+ 3,IF(H157="Medium",#REF!+ 7,IF(H157="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="158" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I158" t="str">
         <f>IF(H158="Hard",#REF!+ 3,IF(H158="Medium",#REF!+ 7,IF(H158="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="159" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I159" t="str">
         <f>IF(H159="Hard",#REF!+ 3,IF(H159="Medium",#REF!+ 7,IF(H159="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="160" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I160" t="str">
         <f>IF(H160="Hard",#REF!+ 3,IF(H160="Medium",#REF!+ 7,IF(H160="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="161" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I161" t="str">
         <f>IF(H161="Hard",#REF!+ 3,IF(H161="Medium",#REF!+ 7,IF(H161="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="162" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I162" t="str">
         <f>IF(H162="Hard",#REF!+ 3,IF(H162="Medium",#REF!+ 7,IF(H162="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="163" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I163" t="str">
         <f>IF(H163="Hard",#REF!+ 3,IF(H163="Medium",#REF!+ 7,IF(H163="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="164" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I164" t="str">
         <f>IF(H164="Hard",#REF!+ 3,IF(H164="Medium",#REF!+ 7,IF(H164="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="165" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I165" t="str">
         <f>IF(H165="Hard",#REF!+ 3,IF(H165="Medium",#REF!+ 7,IF(H165="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="166" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I166" t="str">
         <f>IF(H166="Hard",#REF!+ 3,IF(H166="Medium",#REF!+ 7,IF(H166="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="167" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I167" t="str">
         <f>IF(H167="Hard",#REF!+ 3,IF(H167="Medium",#REF!+ 7,IF(H167="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="168" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I168" t="str">
         <f>IF(H168="Hard",#REF!+ 3,IF(H168="Medium",#REF!+ 7,IF(H168="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="169" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I169" t="str">
         <f>IF(H169="Hard",#REF!+ 3,IF(H169="Medium",#REF!+ 7,IF(H169="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="170" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I170" t="str">
         <f>IF(H170="Hard",#REF!+ 3,IF(H170="Medium",#REF!+ 7,IF(H170="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="171" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I171" t="str">
         <f>IF(H171="Hard",#REF!+ 3,IF(H171="Medium",#REF!+ 7,IF(H171="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="172" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I172" t="str">
         <f>IF(H172="Hard",#REF!+ 3,IF(H172="Medium",#REF!+ 7,IF(H172="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="173" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I173" t="str">
         <f>IF(H173="Hard",#REF!+ 3,IF(H173="Medium",#REF!+ 7,IF(H173="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="174" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I174" t="str">
         <f>IF(H174="Hard",#REF!+ 3,IF(H174="Medium",#REF!+ 7,IF(H174="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="175" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I175" t="str">
         <f>IF(H175="Hard",#REF!+ 3,IF(H175="Medium",#REF!+ 7,IF(H175="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="176" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I176" t="str">
         <f>IF(H176="Hard",#REF!+ 3,IF(H176="Medium",#REF!+ 7,IF(H176="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="177" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I177" t="str">
         <f>IF(H177="Hard",#REF!+ 3,IF(H177="Medium",#REF!+ 7,IF(H177="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="178" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I178" t="str">
         <f>IF(H178="Hard",#REF!+ 3,IF(H178="Medium",#REF!+ 7,IF(H178="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="179" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I179" t="str">
         <f>IF(H179="Hard",#REF!+ 3,IF(H179="Medium",#REF!+ 7,IF(H179="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="180" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I180" t="str">
         <f>IF(H180="Hard",#REF!+ 3,IF(H180="Medium",#REF!+ 7,IF(H180="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="181" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I181" t="str">
         <f>IF(H181="Hard",#REF!+ 3,IF(H181="Medium",#REF!+ 7,IF(H181="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I182" t="str">
         <f>IF(H182="Hard",#REF!+ 3,IF(H182="Medium",#REF!+ 7,IF(H182="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="183" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I183" t="str">
         <f>IF(H183="Hard",#REF!+ 3,IF(H183="Medium",#REF!+ 7,IF(H183="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I184" t="str">
         <f>IF(H184="Hard",#REF!+ 3,IF(H184="Medium",#REF!+ 7,IF(H184="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I185" t="str">
         <f>IF(H185="Hard",#REF!+ 3,IF(H185="Medium",#REF!+ 7,IF(H185="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I186" t="str">
         <f>IF(H186="Hard",#REF!+ 3,IF(H186="Medium",#REF!+ 7,IF(H186="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="187" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I187" t="str">
         <f>IF(H187="Hard",#REF!+ 3,IF(H187="Medium",#REF!+ 7,IF(H187="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="188" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I188" t="str">
         <f>IF(H188="Hard",#REF!+ 3,IF(H188="Medium",#REF!+ 7,IF(H188="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="189" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I189" t="str">
         <f>IF(H189="Hard",#REF!+ 3,IF(H189="Medium",#REF!+ 7,IF(H189="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="190" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I190" t="str">
         <f>IF(H190="Hard",#REF!+ 3,IF(H190="Medium",#REF!+ 7,IF(H190="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="191" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I191" t="str">
         <f>IF(H191="Hard",#REF!+ 3,IF(H191="Medium",#REF!+ 7,IF(H191="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="192" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I192" t="str">
         <f>IF(H192="Hard",#REF!+ 3,IF(H192="Medium",#REF!+ 7,IF(H192="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="193" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I193" t="str">
         <f>IF(H193="Hard",#REF!+ 3,IF(H193="Medium",#REF!+ 7,IF(H193="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="194" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I194" t="str">
         <f>IF(H194="Hard",#REF!+ 3,IF(H194="Medium",#REF!+ 7,IF(H194="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="195" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I195" t="str">
         <f>IF(H195="Hard",#REF!+ 3,IF(H195="Medium",#REF!+ 7,IF(H195="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="196" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I196" t="str">
         <f>IF(H196="Hard",#REF!+ 3,IF(H196="Medium",#REF!+ 7,IF(H196="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="197" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I197" t="str">
         <f>IF(H197="Hard",#REF!+ 3,IF(H197="Medium",#REF!+ 7,IF(H197="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="198" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I198" t="str">
         <f>IF(H198="Hard",#REF!+ 3,IF(H198="Medium",#REF!+ 7,IF(H198="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="199" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I199" t="str">
         <f>IF(H199="Hard",#REF!+ 3,IF(H199="Medium",#REF!+ 7,IF(H199="Easy",#REF!+ 30,"")))</f>
         <v/>
@@ -3485,21 +3596,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3528,346 +3639,653 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2">
         <v>283</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>151</v>
       </c>
       <c r="I2" s="14">
         <v>46052</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>156</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>157</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I3" s="14">
         <v>46041</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I4" s="14">
         <v>46041</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5">
         <v>75</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I5" s="14">
         <v>46041</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6">
         <v>169</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I6" s="14">
         <v>46041</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7">
         <v>53</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I7" s="14">
         <v>46037</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8">
         <v>121</v>
       </c>
       <c r="D8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G8" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I8" s="14">
         <v>46041</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C9">
         <v>560</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G9" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I9" s="14">
         <v>46041</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10">
         <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I10" s="14">
         <v>46041</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C11">
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I11" s="14">
         <v>46037</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C12">
         <v>128</v>
       </c>
       <c r="D12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I12" s="14">
         <v>46040</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C13">
         <v>118</v>
       </c>
       <c r="D13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="I13" s="14">
         <v>46040</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14">
+        <v>229</v>
+      </c>
+      <c r="D14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>191</v>
+      </c>
+      <c r="G14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" s="14">
+        <v>46042</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>195</v>
+      </c>
+      <c r="G15" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" s="14">
+        <v>46038</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" s="14">
+        <v>46038</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
+        <v>200</v>
+      </c>
+      <c r="G17" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I17" s="14">
+        <v>46042</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" t="s">
+        <v>203</v>
+      </c>
+      <c r="G18" t="s">
+        <v>157</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I18" s="14">
+        <v>46042</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>204</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
+        <v>130</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I19" s="14">
+        <v>46042</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20">
+        <v>88</v>
+      </c>
+      <c r="D20" t="s">
+        <v>207</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I20" s="14">
+        <v>46038</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>208</v>
+      </c>
+      <c r="D21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
+        <v>209</v>
+      </c>
+      <c r="G21" t="s">
+        <v>157</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I21" s="14">
+        <v>46039</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
+        <v>213</v>
+      </c>
+      <c r="G22" t="s">
+        <v>157</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" s="14">
+        <v>46039</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C23">
+        <v>493</v>
+      </c>
+      <c r="D23" t="s">
+        <v>215</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I23" s="14">
+        <v>46039</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C24">
+        <v>152</v>
+      </c>
+      <c r="D24" t="s">
+        <v>218</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>130</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I24" s="14">
+        <v>46039</v>
       </c>
     </row>
   </sheetData>
@@ -3878,6 +4296,8 @@
     <hyperlink ref="D6" r:id="rId4" xr:uid="{1A1F4847-2763-4D4C-B18C-7C66F9415C06}"/>
     <hyperlink ref="D5" r:id="rId5" xr:uid="{5D75CC5B-790A-4135-9505-78843D9EC616}"/>
     <hyperlink ref="D7" r:id="rId6" xr:uid="{47EE779C-1BE0-4B40-9A27-5425F3C420B2}"/>
+    <hyperlink ref="D15" r:id="rId7" xr:uid="{B38188FE-686A-42CA-B79C-2304C3736E4D}"/>
+    <hyperlink ref="D22" r:id="rId8" xr:uid="{E615E439-7F0D-4061-9A54-10A905E94EAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added latest DSA Revision Tracker
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87016EE6-55B6-4D6D-B7DA-756954558137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D7AC59-DCAD-456A-93F8-43650EC48C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1129,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2548,7 +2548,7 @@
       <c r="C45">
         <v>1922</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="10" t="s">
         <v>141</v>
       </c>
       <c r="E45" s="11" t="s">
@@ -3589,6 +3589,7 @@
     <hyperlink ref="D46" r:id="rId3" xr:uid="{6EF8B0EF-27B5-4A6C-8FAA-8D8FFF890651}"/>
     <hyperlink ref="D47" r:id="rId4" xr:uid="{33F92BC2-1EF1-499C-BFC6-6432476C5EF5}"/>
     <hyperlink ref="D48" r:id="rId5" xr:uid="{F67762AC-77CD-4EF5-AC97-5E4313FB66FA}"/>
+    <hyperlink ref="D45" r:id="rId6" xr:uid="{DA15E00B-9E05-44E5-B99F-2D23160E68D0}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3599,7 +3600,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added some more solutions from arrays topic
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D7AC59-DCAD-456A-93F8-43650EC48C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04E39B5-211E-47EE-B977-6D44CBD62AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA Tracker" sheetId="1" r:id="rId1"/>
@@ -1129,21 +1129,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView topLeftCell="A16" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.54296875" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
-    <col min="6" max="6" width="33.1796875" customWidth="1"/>
-    <col min="7" max="7" width="17.54296875" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>46065</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1273,7 +1273,7 @@
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1343,7 +1343,7 @@
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1381,7 +1381,7 @@
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1454,7 +1454,7 @@
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1492,7 +1492,7 @@
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1530,7 +1530,7 @@
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1565,7 +1565,7 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1603,7 +1603,7 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1641,7 +1641,7 @@
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1679,7 +1679,7 @@
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1717,7 +1717,7 @@
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1755,7 +1755,7 @@
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1784,7 +1784,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1816,7 +1816,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1845,7 +1845,7 @@
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1909,7 +1909,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1938,7 +1938,7 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1967,7 +1967,7 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1996,7 +1996,7 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2028,7 +2028,7 @@
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2060,7 +2060,7 @@
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2092,7 +2092,7 @@
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2124,7 +2124,7 @@
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2156,7 +2156,7 @@
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="Q31" s="15"/>
       <c r="R31" s="15"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2217,7 +2217,7 @@
       <c r="Q32" s="15"/>
       <c r="R32" s="15"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2249,7 +2249,7 @@
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="Q34" s="15"/>
       <c r="R34" s="15"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2313,7 +2313,7 @@
       <c r="Q35" s="15"/>
       <c r="R35" s="15"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>46040</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>46038</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2703,877 +2703,877 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I54" t="str">
         <f>IF(H54="Hard",#REF!+ 3,IF(H54="Medium",#REF!+ 7,IF(H54="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I55" t="str">
         <f>IF(H55="Hard",#REF!+ 3,IF(H55="Medium",#REF!+ 7,IF(H55="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I56" t="str">
         <f>IF(H56="Hard",#REF!+ 3,IF(H56="Medium",#REF!+ 7,IF(H56="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I57" t="str">
         <f>IF(H57="Hard",#REF!+ 3,IF(H57="Medium",#REF!+ 7,IF(H57="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I58" t="str">
         <f>IF(H58="Hard",#REF!+ 3,IF(H58="Medium",#REF!+ 7,IF(H58="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I59" t="str">
         <f>IF(H59="Hard",#REF!+ 3,IF(H59="Medium",#REF!+ 7,IF(H59="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I60" t="str">
         <f>IF(H60="Hard",#REF!+ 3,IF(H60="Medium",#REF!+ 7,IF(H60="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I61" t="str">
         <f>IF(H61="Hard",#REF!+ 3,IF(H61="Medium",#REF!+ 7,IF(H61="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I62" t="str">
         <f>IF(H62="Hard",#REF!+ 3,IF(H62="Medium",#REF!+ 7,IF(H62="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I63" t="str">
         <f>IF(H63="Hard",#REF!+ 3,IF(H63="Medium",#REF!+ 7,IF(H63="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I64" t="str">
         <f>IF(H64="Hard",#REF!+ 3,IF(H64="Medium",#REF!+ 7,IF(H64="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I65" t="str">
         <f>IF(H65="Hard",#REF!+ 3,IF(H65="Medium",#REF!+ 7,IF(H65="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I66" t="str">
         <f>IF(H66="Hard",#REF!+ 3,IF(H66="Medium",#REF!+ 7,IF(H66="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I67" t="str">
         <f>IF(H67="Hard",#REF!+ 3,IF(H67="Medium",#REF!+ 7,IF(H67="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I68" t="str">
         <f>IF(H68="Hard",#REF!+ 3,IF(H68="Medium",#REF!+ 7,IF(H68="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I69" t="str">
         <f>IF(H69="Hard",#REF!+ 3,IF(H69="Medium",#REF!+ 7,IF(H69="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I70" t="str">
         <f>IF(H70="Hard",#REF!+ 3,IF(H70="Medium",#REF!+ 7,IF(H70="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I71" t="str">
         <f>IF(H71="Hard",#REF!+ 3,IF(H71="Medium",#REF!+ 7,IF(H71="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I72" t="str">
         <f>IF(H72="Hard",#REF!+ 3,IF(H72="Medium",#REF!+ 7,IF(H72="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I73" t="str">
         <f>IF(H73="Hard",#REF!+ 3,IF(H73="Medium",#REF!+ 7,IF(H73="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I74" t="str">
         <f>IF(H74="Hard",#REF!+ 3,IF(H74="Medium",#REF!+ 7,IF(H74="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I75" t="str">
         <f>IF(H75="Hard",#REF!+ 3,IF(H75="Medium",#REF!+ 7,IF(H75="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I76" t="str">
         <f>IF(H76="Hard",#REF!+ 3,IF(H76="Medium",#REF!+ 7,IF(H76="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I77" t="str">
         <f>IF(H77="Hard",#REF!+ 3,IF(H77="Medium",#REF!+ 7,IF(H77="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I78" t="str">
         <f>IF(H78="Hard",#REF!+ 3,IF(H78="Medium",#REF!+ 7,IF(H78="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I79" t="str">
         <f>IF(H79="Hard",#REF!+ 3,IF(H79="Medium",#REF!+ 7,IF(H79="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I80" t="str">
         <f>IF(H80="Hard",#REF!+ 3,IF(H80="Medium",#REF!+ 7,IF(H80="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I81" t="str">
         <f>IF(H81="Hard",#REF!+ 3,IF(H81="Medium",#REF!+ 7,IF(H81="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I82" t="str">
         <f>IF(H82="Hard",#REF!+ 3,IF(H82="Medium",#REF!+ 7,IF(H82="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I83" t="str">
         <f>IF(H83="Hard",#REF!+ 3,IF(H83="Medium",#REF!+ 7,IF(H83="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I84" t="str">
         <f>IF(H84="Hard",#REF!+ 3,IF(H84="Medium",#REF!+ 7,IF(H84="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I85" t="str">
         <f>IF(H85="Hard",#REF!+ 3,IF(H85="Medium",#REF!+ 7,IF(H85="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I86" t="str">
         <f>IF(H86="Hard",#REF!+ 3,IF(H86="Medium",#REF!+ 7,IF(H86="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I87" t="str">
         <f>IF(H87="Hard",#REF!+ 3,IF(H87="Medium",#REF!+ 7,IF(H87="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I88" t="str">
         <f>IF(H88="Hard",#REF!+ 3,IF(H88="Medium",#REF!+ 7,IF(H88="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I89" t="str">
         <f>IF(H89="Hard",#REF!+ 3,IF(H89="Medium",#REF!+ 7,IF(H89="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I90" t="str">
         <f>IF(H90="Hard",#REF!+ 3,IF(H90="Medium",#REF!+ 7,IF(H90="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I91" t="str">
         <f>IF(H91="Hard",#REF!+ 3,IF(H91="Medium",#REF!+ 7,IF(H91="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I92" t="str">
         <f>IF(H92="Hard",#REF!+ 3,IF(H92="Medium",#REF!+ 7,IF(H92="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I93" t="str">
         <f>IF(H93="Hard",#REF!+ 3,IF(H93="Medium",#REF!+ 7,IF(H93="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I94" t="str">
         <f>IF(H94="Hard",#REF!+ 3,IF(H94="Medium",#REF!+ 7,IF(H94="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I95" t="str">
         <f>IF(H95="Hard",#REF!+ 3,IF(H95="Medium",#REF!+ 7,IF(H95="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I96" t="str">
         <f>IF(H96="Hard",#REF!+ 3,IF(H96="Medium",#REF!+ 7,IF(H96="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I97" t="str">
         <f>IF(H97="Hard",#REF!+ 3,IF(H97="Medium",#REF!+ 7,IF(H97="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I98" t="str">
         <f>IF(H98="Hard",#REF!+ 3,IF(H98="Medium",#REF!+ 7,IF(H98="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I99" t="str">
         <f>IF(H99="Hard",#REF!+ 3,IF(H99="Medium",#REF!+ 7,IF(H99="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I100" t="str">
         <f>IF(H100="Hard",#REF!+ 3,IF(H100="Medium",#REF!+ 7,IF(H100="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I101" t="str">
         <f>IF(H101="Hard",#REF!+ 3,IF(H101="Medium",#REF!+ 7,IF(H101="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I102" t="str">
         <f>IF(H102="Hard",#REF!+ 3,IF(H102="Medium",#REF!+ 7,IF(H102="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I103" t="str">
         <f>IF(H103="Hard",#REF!+ 3,IF(H103="Medium",#REF!+ 7,IF(H103="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I104" t="str">
         <f>IF(H104="Hard",#REF!+ 3,IF(H104="Medium",#REF!+ 7,IF(H104="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I105" t="str">
         <f>IF(H105="Hard",#REF!+ 3,IF(H105="Medium",#REF!+ 7,IF(H105="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I106" t="str">
         <f>IF(H106="Hard",#REF!+ 3,IF(H106="Medium",#REF!+ 7,IF(H106="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I107" t="str">
         <f>IF(H107="Hard",#REF!+ 3,IF(H107="Medium",#REF!+ 7,IF(H107="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I108" t="str">
         <f>IF(H108="Hard",#REF!+ 3,IF(H108="Medium",#REF!+ 7,IF(H108="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="109" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I109" t="str">
         <f>IF(H109="Hard",#REF!+ 3,IF(H109="Medium",#REF!+ 7,IF(H109="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="110" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I110" t="str">
         <f>IF(H110="Hard",#REF!+ 3,IF(H110="Medium",#REF!+ 7,IF(H110="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="111" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I111" t="str">
         <f>IF(H111="Hard",#REF!+ 3,IF(H111="Medium",#REF!+ 7,IF(H111="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="112" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I112" t="str">
         <f>IF(H112="Hard",#REF!+ 3,IF(H112="Medium",#REF!+ 7,IF(H112="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="113" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I113" t="str">
         <f>IF(H113="Hard",#REF!+ 3,IF(H113="Medium",#REF!+ 7,IF(H113="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="114" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I114" t="str">
         <f>IF(H114="Hard",#REF!+ 3,IF(H114="Medium",#REF!+ 7,IF(H114="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I115" t="str">
         <f>IF(H115="Hard",#REF!+ 3,IF(H115="Medium",#REF!+ 7,IF(H115="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="116" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I116" t="str">
         <f>IF(H116="Hard",#REF!+ 3,IF(H116="Medium",#REF!+ 7,IF(H116="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="117" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I117" t="str">
         <f>IF(H117="Hard",#REF!+ 3,IF(H117="Medium",#REF!+ 7,IF(H117="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="118" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I118" t="str">
         <f>IF(H118="Hard",#REF!+ 3,IF(H118="Medium",#REF!+ 7,IF(H118="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="119" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I119" t="str">
         <f>IF(H119="Hard",#REF!+ 3,IF(H119="Medium",#REF!+ 7,IF(H119="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="120" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I120" t="str">
         <f>IF(H120="Hard",#REF!+ 3,IF(H120="Medium",#REF!+ 7,IF(H120="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="121" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I121" t="str">
         <f>IF(H121="Hard",#REF!+ 3,IF(H121="Medium",#REF!+ 7,IF(H121="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="122" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I122" t="str">
         <f>IF(H122="Hard",#REF!+ 3,IF(H122="Medium",#REF!+ 7,IF(H122="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="123" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I123" t="str">
         <f>IF(H123="Hard",#REF!+ 3,IF(H123="Medium",#REF!+ 7,IF(H123="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="124" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I124" t="str">
         <f>IF(H124="Hard",#REF!+ 3,IF(H124="Medium",#REF!+ 7,IF(H124="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="125" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I125" t="str">
         <f>IF(H125="Hard",#REF!+ 3,IF(H125="Medium",#REF!+ 7,IF(H125="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="126" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I126" t="str">
         <f>IF(H126="Hard",#REF!+ 3,IF(H126="Medium",#REF!+ 7,IF(H126="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="127" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I127" t="str">
         <f>IF(H127="Hard",#REF!+ 3,IF(H127="Medium",#REF!+ 7,IF(H127="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="128" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I128" t="str">
         <f>IF(H128="Hard",#REF!+ 3,IF(H128="Medium",#REF!+ 7,IF(H128="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="129" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I129" t="str">
         <f>IF(H129="Hard",#REF!+ 3,IF(H129="Medium",#REF!+ 7,IF(H129="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="130" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I130" t="str">
         <f>IF(H130="Hard",#REF!+ 3,IF(H130="Medium",#REF!+ 7,IF(H130="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I131" t="str">
         <f>IF(H131="Hard",#REF!+ 3,IF(H131="Medium",#REF!+ 7,IF(H131="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I132" t="str">
         <f>IF(H132="Hard",#REF!+ 3,IF(H132="Medium",#REF!+ 7,IF(H132="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="133" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I133" t="str">
         <f>IF(H133="Hard",#REF!+ 3,IF(H133="Medium",#REF!+ 7,IF(H133="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="134" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I134" t="str">
         <f>IF(H134="Hard",#REF!+ 3,IF(H134="Medium",#REF!+ 7,IF(H134="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="135" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I135" t="str">
         <f>IF(H135="Hard",#REF!+ 3,IF(H135="Medium",#REF!+ 7,IF(H135="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="136" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I136" t="str">
         <f>IF(H136="Hard",#REF!+ 3,IF(H136="Medium",#REF!+ 7,IF(H136="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="137" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I137" t="str">
         <f>IF(H137="Hard",#REF!+ 3,IF(H137="Medium",#REF!+ 7,IF(H137="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="138" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I138" t="str">
         <f>IF(H138="Hard",#REF!+ 3,IF(H138="Medium",#REF!+ 7,IF(H138="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="139" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I139" t="str">
         <f>IF(H139="Hard",#REF!+ 3,IF(H139="Medium",#REF!+ 7,IF(H139="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="140" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I140" t="str">
         <f>IF(H140="Hard",#REF!+ 3,IF(H140="Medium",#REF!+ 7,IF(H140="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="141" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I141" t="str">
         <f>IF(H141="Hard",#REF!+ 3,IF(H141="Medium",#REF!+ 7,IF(H141="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="142" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I142" t="str">
         <f>IF(H142="Hard",#REF!+ 3,IF(H142="Medium",#REF!+ 7,IF(H142="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="143" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I143" t="str">
         <f>IF(H143="Hard",#REF!+ 3,IF(H143="Medium",#REF!+ 7,IF(H143="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="144" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I144" t="str">
         <f>IF(H144="Hard",#REF!+ 3,IF(H144="Medium",#REF!+ 7,IF(H144="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="145" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I145" t="str">
         <f>IF(H145="Hard",#REF!+ 3,IF(H145="Medium",#REF!+ 7,IF(H145="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="146" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I146" t="str">
         <f>IF(H146="Hard",#REF!+ 3,IF(H146="Medium",#REF!+ 7,IF(H146="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="147" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I147" t="str">
         <f>IF(H147="Hard",#REF!+ 3,IF(H147="Medium",#REF!+ 7,IF(H147="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="148" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I148" t="str">
         <f>IF(H148="Hard",#REF!+ 3,IF(H148="Medium",#REF!+ 7,IF(H148="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="149" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I149" t="str">
         <f>IF(H149="Hard",#REF!+ 3,IF(H149="Medium",#REF!+ 7,IF(H149="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="150" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I150" t="str">
         <f>IF(H150="Hard",#REF!+ 3,IF(H150="Medium",#REF!+ 7,IF(H150="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="151" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I151" t="str">
         <f>IF(H151="Hard",#REF!+ 3,IF(H151="Medium",#REF!+ 7,IF(H151="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="152" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I152" t="str">
         <f>IF(H152="Hard",#REF!+ 3,IF(H152="Medium",#REF!+ 7,IF(H152="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="153" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I153" t="str">
         <f>IF(H153="Hard",#REF!+ 3,IF(H153="Medium",#REF!+ 7,IF(H153="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="154" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I154" t="str">
         <f>IF(H154="Hard",#REF!+ 3,IF(H154="Medium",#REF!+ 7,IF(H154="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="155" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I155" t="str">
         <f>IF(H155="Hard",#REF!+ 3,IF(H155="Medium",#REF!+ 7,IF(H155="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="156" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I156" t="str">
         <f>IF(H156="Hard",#REF!+ 3,IF(H156="Medium",#REF!+ 7,IF(H156="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="157" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I157" t="str">
         <f>IF(H157="Hard",#REF!+ 3,IF(H157="Medium",#REF!+ 7,IF(H157="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="158" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I158" t="str">
         <f>IF(H158="Hard",#REF!+ 3,IF(H158="Medium",#REF!+ 7,IF(H158="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="159" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I159" t="str">
         <f>IF(H159="Hard",#REF!+ 3,IF(H159="Medium",#REF!+ 7,IF(H159="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="160" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I160" t="str">
         <f>IF(H160="Hard",#REF!+ 3,IF(H160="Medium",#REF!+ 7,IF(H160="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="161" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I161" t="str">
         <f>IF(H161="Hard",#REF!+ 3,IF(H161="Medium",#REF!+ 7,IF(H161="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="162" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="162" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I162" t="str">
         <f>IF(H162="Hard",#REF!+ 3,IF(H162="Medium",#REF!+ 7,IF(H162="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="163" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="163" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I163" t="str">
         <f>IF(H163="Hard",#REF!+ 3,IF(H163="Medium",#REF!+ 7,IF(H163="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="164" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="164" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I164" t="str">
         <f>IF(H164="Hard",#REF!+ 3,IF(H164="Medium",#REF!+ 7,IF(H164="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="165" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="165" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I165" t="str">
         <f>IF(H165="Hard",#REF!+ 3,IF(H165="Medium",#REF!+ 7,IF(H165="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="166" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="166" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I166" t="str">
         <f>IF(H166="Hard",#REF!+ 3,IF(H166="Medium",#REF!+ 7,IF(H166="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="167" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I167" t="str">
         <f>IF(H167="Hard",#REF!+ 3,IF(H167="Medium",#REF!+ 7,IF(H167="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="168" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="168" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I168" t="str">
         <f>IF(H168="Hard",#REF!+ 3,IF(H168="Medium",#REF!+ 7,IF(H168="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="169" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I169" t="str">
         <f>IF(H169="Hard",#REF!+ 3,IF(H169="Medium",#REF!+ 7,IF(H169="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="170" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="170" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I170" t="str">
         <f>IF(H170="Hard",#REF!+ 3,IF(H170="Medium",#REF!+ 7,IF(H170="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="171" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="171" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I171" t="str">
         <f>IF(H171="Hard",#REF!+ 3,IF(H171="Medium",#REF!+ 7,IF(H171="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="172" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="172" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I172" t="str">
         <f>IF(H172="Hard",#REF!+ 3,IF(H172="Medium",#REF!+ 7,IF(H172="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="173" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="173" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I173" t="str">
         <f>IF(H173="Hard",#REF!+ 3,IF(H173="Medium",#REF!+ 7,IF(H173="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="174" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="174" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I174" t="str">
         <f>IF(H174="Hard",#REF!+ 3,IF(H174="Medium",#REF!+ 7,IF(H174="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="175" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="175" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I175" t="str">
         <f>IF(H175="Hard",#REF!+ 3,IF(H175="Medium",#REF!+ 7,IF(H175="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="176" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="176" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I176" t="str">
         <f>IF(H176="Hard",#REF!+ 3,IF(H176="Medium",#REF!+ 7,IF(H176="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="177" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I177" t="str">
         <f>IF(H177="Hard",#REF!+ 3,IF(H177="Medium",#REF!+ 7,IF(H177="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="178" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I178" t="str">
         <f>IF(H178="Hard",#REF!+ 3,IF(H178="Medium",#REF!+ 7,IF(H178="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="179" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I179" t="str">
         <f>IF(H179="Hard",#REF!+ 3,IF(H179="Medium",#REF!+ 7,IF(H179="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="180" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I180" t="str">
         <f>IF(H180="Hard",#REF!+ 3,IF(H180="Medium",#REF!+ 7,IF(H180="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="181" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="181" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I181" t="str">
         <f>IF(H181="Hard",#REF!+ 3,IF(H181="Medium",#REF!+ 7,IF(H181="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="182" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I182" t="str">
         <f>IF(H182="Hard",#REF!+ 3,IF(H182="Medium",#REF!+ 7,IF(H182="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="183" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="183" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I183" t="str">
         <f>IF(H183="Hard",#REF!+ 3,IF(H183="Medium",#REF!+ 7,IF(H183="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="184" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I184" t="str">
         <f>IF(H184="Hard",#REF!+ 3,IF(H184="Medium",#REF!+ 7,IF(H184="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I185" t="str">
         <f>IF(H185="Hard",#REF!+ 3,IF(H185="Medium",#REF!+ 7,IF(H185="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="186" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I186" t="str">
         <f>IF(H186="Hard",#REF!+ 3,IF(H186="Medium",#REF!+ 7,IF(H186="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="187" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="187" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I187" t="str">
         <f>IF(H187="Hard",#REF!+ 3,IF(H187="Medium",#REF!+ 7,IF(H187="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="188" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I188" t="str">
         <f>IF(H188="Hard",#REF!+ 3,IF(H188="Medium",#REF!+ 7,IF(H188="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="189" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I189" t="str">
         <f>IF(H189="Hard",#REF!+ 3,IF(H189="Medium",#REF!+ 7,IF(H189="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="190" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I190" t="str">
         <f>IF(H190="Hard",#REF!+ 3,IF(H190="Medium",#REF!+ 7,IF(H190="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="191" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="191" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I191" t="str">
         <f>IF(H191="Hard",#REF!+ 3,IF(H191="Medium",#REF!+ 7,IF(H191="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="192" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="192" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I192" t="str">
         <f>IF(H192="Hard",#REF!+ 3,IF(H192="Medium",#REF!+ 7,IF(H192="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="193" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I193" t="str">
         <f>IF(H193="Hard",#REF!+ 3,IF(H193="Medium",#REF!+ 7,IF(H193="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="194" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="194" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I194" t="str">
         <f>IF(H194="Hard",#REF!+ 3,IF(H194="Medium",#REF!+ 7,IF(H194="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="195" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="195" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I195" t="str">
         <f>IF(H195="Hard",#REF!+ 3,IF(H195="Medium",#REF!+ 7,IF(H195="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="196" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I196" t="str">
         <f>IF(H196="Hard",#REF!+ 3,IF(H196="Medium",#REF!+ 7,IF(H196="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="197" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="197" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I197" t="str">
         <f>IF(H197="Hard",#REF!+ 3,IF(H197="Medium",#REF!+ 7,IF(H197="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="198" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="198" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I198" t="str">
         <f>IF(H198="Hard",#REF!+ 3,IF(H198="Medium",#REF!+ 7,IF(H198="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="199" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="199" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I199" t="str">
         <f>IF(H199="Hard",#REF!+ 3,IF(H199="Medium",#REF!+ 7,IF(H199="Easy",#REF!+ 30,"")))</f>
         <v/>
@@ -3600,18 +3600,18 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>46052</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3801,14 +3801,14 @@
       <c r="G7" t="s">
         <v>130</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>138</v>
+      <c r="H7" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I7" s="14">
-        <v>46037</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3917,14 +3917,14 @@
       <c r="G11" t="s">
         <v>130</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>138</v>
+      <c r="H11" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I11" s="14">
-        <v>46037</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46044</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>46040</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>46040</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4033,14 +4033,14 @@
       <c r="G15" t="s">
         <v>130</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>138</v>
+      <c r="H15" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I15" s="14">
-        <v>46038</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46044</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4062,14 +4062,14 @@
       <c r="G16" t="s">
         <v>130</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>138</v>
+      <c r="H16" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I16" s="14">
-        <v>46038</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46044</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4172,14 +4172,14 @@
       <c r="G20" t="s">
         <v>130</v>
       </c>
-      <c r="H20" s="12" t="s">
-        <v>138</v>
+      <c r="H20" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I20" s="14">
-        <v>46038</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46044</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Added solutions for new recurssion problems
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04E39B5-211E-47EE-B977-6D44CBD62AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44076F20-7451-4FED-AB2D-7080068F2F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA Tracker" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="231">
   <si>
     <t>ID</t>
   </si>
@@ -689,6 +689,42 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/maximum-product-subarray/description/</t>
+  </si>
+  <si>
+    <t>Power(x, n)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/powx-n/</t>
+  </si>
+  <si>
+    <t>Recursion, Edge Case</t>
+  </si>
+  <si>
+    <t>Count all subsequence with sum k</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/count-all-subsequences-with-sum-k</t>
+  </si>
+  <si>
+    <t>Check if there exists a subsequence with sum k</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/check-if-there-exists-a-subsequence-with-sum-k</t>
+  </si>
+  <si>
+    <t>Recursion, take not take</t>
+  </si>
+  <si>
+    <t>Combination sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum/description/</t>
+  </si>
+  <si>
+    <t>Combination sum 2</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum-ii/description/</t>
   </si>
 </sst>
 </file>
@@ -724,7 +760,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -791,6 +827,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -805,7 +847,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -821,6 +863,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1129,21 +1172,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A41" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" customWidth="1"/>
+    <col min="6" max="6" width="33.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1198,7 +1241,7 @@
         <v>46065</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1226,19 +1269,19 @@
       <c r="I3" s="14">
         <v>46065</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1263,17 +1306,17 @@
       <c r="I4" s="14">
         <v>46065</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1298,17 +1341,17 @@
       <c r="I5" s="14">
         <v>46065</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1333,17 +1376,17 @@
       <c r="I6" s="14">
         <v>46065</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1371,17 +1414,17 @@
       <c r="I7" s="14">
         <v>46065</v>
       </c>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1406,17 +1449,17 @@
       <c r="I8" s="14">
         <v>46040</v>
       </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1444,17 +1487,17 @@
       <c r="I9" s="14">
         <v>46036</v>
       </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1482,17 +1525,17 @@
       <c r="I10" s="14">
         <v>46065</v>
       </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1520,17 +1563,17 @@
       <c r="I11" s="14">
         <v>46065</v>
       </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1555,17 +1598,17 @@
       <c r="I12" s="14">
         <v>46065</v>
       </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1593,17 +1636,17 @@
       <c r="I13" s="14">
         <v>46065</v>
       </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1631,17 +1674,17 @@
       <c r="I14" s="14">
         <v>46041</v>
       </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1669,17 +1712,17 @@
       <c r="I15" s="14">
         <v>46066</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1707,17 +1750,17 @@
       <c r="I16" s="14">
         <v>46066</v>
       </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1745,17 +1788,17 @@
       <c r="I17" s="14">
         <v>46066</v>
       </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1774,17 +1817,17 @@
       <c r="G18" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1806,17 +1849,17 @@
       <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1835,17 +1878,17 @@
       <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1867,17 +1910,17 @@
       <c r="G21" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1899,17 +1942,17 @@
       <c r="G22" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1928,17 +1971,17 @@
       <c r="G23" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1957,17 +2000,17 @@
       <c r="G24" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1986,17 +2029,17 @@
       <c r="G25" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2018,17 +2061,17 @@
       <c r="G26" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2050,17 +2093,17 @@
       <c r="G27" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2082,17 +2125,17 @@
       <c r="G28" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2114,17 +2157,17 @@
       <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2146,17 +2189,17 @@
       <c r="G30" t="s">
         <v>74</v>
       </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2175,17 +2218,17 @@
       <c r="G31" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2207,17 +2250,17 @@
       <c r="G32" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2239,17 +2282,17 @@
       <c r="G33" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2271,17 +2314,17 @@
       <c r="G34" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2303,17 +2346,17 @@
       <c r="G35" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2336,7 +2379,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2359,7 +2402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2382,7 +2425,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2405,7 +2448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2428,7 +2471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2451,7 +2494,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2480,7 +2523,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2509,7 +2552,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2538,7 +2581,7 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2567,7 +2610,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2593,7 +2636,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2619,7 +2662,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2645,7 +2688,7 @@
         <v>46040</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2674,7 +2717,7 @@
         <v>46038</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2703,877 +2746,877 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I54" t="str">
         <f>IF(H54="Hard",#REF!+ 3,IF(H54="Medium",#REF!+ 7,IF(H54="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I55" t="str">
         <f>IF(H55="Hard",#REF!+ 3,IF(H55="Medium",#REF!+ 7,IF(H55="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I56" t="str">
         <f>IF(H56="Hard",#REF!+ 3,IF(H56="Medium",#REF!+ 7,IF(H56="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I57" t="str">
         <f>IF(H57="Hard",#REF!+ 3,IF(H57="Medium",#REF!+ 7,IF(H57="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I58" t="str">
         <f>IF(H58="Hard",#REF!+ 3,IF(H58="Medium",#REF!+ 7,IF(H58="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I59" t="str">
         <f>IF(H59="Hard",#REF!+ 3,IF(H59="Medium",#REF!+ 7,IF(H59="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I60" t="str">
         <f>IF(H60="Hard",#REF!+ 3,IF(H60="Medium",#REF!+ 7,IF(H60="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I61" t="str">
         <f>IF(H61="Hard",#REF!+ 3,IF(H61="Medium",#REF!+ 7,IF(H61="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I62" t="str">
         <f>IF(H62="Hard",#REF!+ 3,IF(H62="Medium",#REF!+ 7,IF(H62="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I63" t="str">
         <f>IF(H63="Hard",#REF!+ 3,IF(H63="Medium",#REF!+ 7,IF(H63="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I64" t="str">
         <f>IF(H64="Hard",#REF!+ 3,IF(H64="Medium",#REF!+ 7,IF(H64="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I65" t="str">
         <f>IF(H65="Hard",#REF!+ 3,IF(H65="Medium",#REF!+ 7,IF(H65="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I66" t="str">
         <f>IF(H66="Hard",#REF!+ 3,IF(H66="Medium",#REF!+ 7,IF(H66="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I67" t="str">
         <f>IF(H67="Hard",#REF!+ 3,IF(H67="Medium",#REF!+ 7,IF(H67="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I68" t="str">
         <f>IF(H68="Hard",#REF!+ 3,IF(H68="Medium",#REF!+ 7,IF(H68="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I69" t="str">
         <f>IF(H69="Hard",#REF!+ 3,IF(H69="Medium",#REF!+ 7,IF(H69="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I70" t="str">
         <f>IF(H70="Hard",#REF!+ 3,IF(H70="Medium",#REF!+ 7,IF(H70="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I71" t="str">
         <f>IF(H71="Hard",#REF!+ 3,IF(H71="Medium",#REF!+ 7,IF(H71="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I72" t="str">
         <f>IF(H72="Hard",#REF!+ 3,IF(H72="Medium",#REF!+ 7,IF(H72="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I73" t="str">
         <f>IF(H73="Hard",#REF!+ 3,IF(H73="Medium",#REF!+ 7,IF(H73="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I74" t="str">
         <f>IF(H74="Hard",#REF!+ 3,IF(H74="Medium",#REF!+ 7,IF(H74="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I75" t="str">
         <f>IF(H75="Hard",#REF!+ 3,IF(H75="Medium",#REF!+ 7,IF(H75="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I76" t="str">
         <f>IF(H76="Hard",#REF!+ 3,IF(H76="Medium",#REF!+ 7,IF(H76="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I77" t="str">
         <f>IF(H77="Hard",#REF!+ 3,IF(H77="Medium",#REF!+ 7,IF(H77="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I78" t="str">
         <f>IF(H78="Hard",#REF!+ 3,IF(H78="Medium",#REF!+ 7,IF(H78="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I79" t="str">
         <f>IF(H79="Hard",#REF!+ 3,IF(H79="Medium",#REF!+ 7,IF(H79="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I80" t="str">
         <f>IF(H80="Hard",#REF!+ 3,IF(H80="Medium",#REF!+ 7,IF(H80="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I81" t="str">
         <f>IF(H81="Hard",#REF!+ 3,IF(H81="Medium",#REF!+ 7,IF(H81="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I82" t="str">
         <f>IF(H82="Hard",#REF!+ 3,IF(H82="Medium",#REF!+ 7,IF(H82="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I83" t="str">
         <f>IF(H83="Hard",#REF!+ 3,IF(H83="Medium",#REF!+ 7,IF(H83="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I84" t="str">
         <f>IF(H84="Hard",#REF!+ 3,IF(H84="Medium",#REF!+ 7,IF(H84="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I85" t="str">
         <f>IF(H85="Hard",#REF!+ 3,IF(H85="Medium",#REF!+ 7,IF(H85="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I86" t="str">
         <f>IF(H86="Hard",#REF!+ 3,IF(H86="Medium",#REF!+ 7,IF(H86="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I87" t="str">
         <f>IF(H87="Hard",#REF!+ 3,IF(H87="Medium",#REF!+ 7,IF(H87="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I88" t="str">
         <f>IF(H88="Hard",#REF!+ 3,IF(H88="Medium",#REF!+ 7,IF(H88="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I89" t="str">
         <f>IF(H89="Hard",#REF!+ 3,IF(H89="Medium",#REF!+ 7,IF(H89="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I90" t="str">
         <f>IF(H90="Hard",#REF!+ 3,IF(H90="Medium",#REF!+ 7,IF(H90="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I91" t="str">
         <f>IF(H91="Hard",#REF!+ 3,IF(H91="Medium",#REF!+ 7,IF(H91="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I92" t="str">
         <f>IF(H92="Hard",#REF!+ 3,IF(H92="Medium",#REF!+ 7,IF(H92="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I93" t="str">
         <f>IF(H93="Hard",#REF!+ 3,IF(H93="Medium",#REF!+ 7,IF(H93="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I94" t="str">
         <f>IF(H94="Hard",#REF!+ 3,IF(H94="Medium",#REF!+ 7,IF(H94="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I95" t="str">
         <f>IF(H95="Hard",#REF!+ 3,IF(H95="Medium",#REF!+ 7,IF(H95="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I96" t="str">
         <f>IF(H96="Hard",#REF!+ 3,IF(H96="Medium",#REF!+ 7,IF(H96="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I97" t="str">
         <f>IF(H97="Hard",#REF!+ 3,IF(H97="Medium",#REF!+ 7,IF(H97="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I98" t="str">
         <f>IF(H98="Hard",#REF!+ 3,IF(H98="Medium",#REF!+ 7,IF(H98="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I99" t="str">
         <f>IF(H99="Hard",#REF!+ 3,IF(H99="Medium",#REF!+ 7,IF(H99="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I100" t="str">
         <f>IF(H100="Hard",#REF!+ 3,IF(H100="Medium",#REF!+ 7,IF(H100="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I101" t="str">
         <f>IF(H101="Hard",#REF!+ 3,IF(H101="Medium",#REF!+ 7,IF(H101="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I102" t="str">
         <f>IF(H102="Hard",#REF!+ 3,IF(H102="Medium",#REF!+ 7,IF(H102="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I103" t="str">
         <f>IF(H103="Hard",#REF!+ 3,IF(H103="Medium",#REF!+ 7,IF(H103="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I104" t="str">
         <f>IF(H104="Hard",#REF!+ 3,IF(H104="Medium",#REF!+ 7,IF(H104="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I105" t="str">
         <f>IF(H105="Hard",#REF!+ 3,IF(H105="Medium",#REF!+ 7,IF(H105="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I106" t="str">
         <f>IF(H106="Hard",#REF!+ 3,IF(H106="Medium",#REF!+ 7,IF(H106="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I107" t="str">
         <f>IF(H107="Hard",#REF!+ 3,IF(H107="Medium",#REF!+ 7,IF(H107="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I108" t="str">
         <f>IF(H108="Hard",#REF!+ 3,IF(H108="Medium",#REF!+ 7,IF(H108="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I109" t="str">
         <f>IF(H109="Hard",#REF!+ 3,IF(H109="Medium",#REF!+ 7,IF(H109="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I110" t="str">
         <f>IF(H110="Hard",#REF!+ 3,IF(H110="Medium",#REF!+ 7,IF(H110="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I111" t="str">
         <f>IF(H111="Hard",#REF!+ 3,IF(H111="Medium",#REF!+ 7,IF(H111="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I112" t="str">
         <f>IF(H112="Hard",#REF!+ 3,IF(H112="Medium",#REF!+ 7,IF(H112="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I113" t="str">
         <f>IF(H113="Hard",#REF!+ 3,IF(H113="Medium",#REF!+ 7,IF(H113="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="114" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I114" t="str">
         <f>IF(H114="Hard",#REF!+ 3,IF(H114="Medium",#REF!+ 7,IF(H114="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I115" t="str">
         <f>IF(H115="Hard",#REF!+ 3,IF(H115="Medium",#REF!+ 7,IF(H115="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="116" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I116" t="str">
         <f>IF(H116="Hard",#REF!+ 3,IF(H116="Medium",#REF!+ 7,IF(H116="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="117" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I117" t="str">
         <f>IF(H117="Hard",#REF!+ 3,IF(H117="Medium",#REF!+ 7,IF(H117="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I118" t="str">
         <f>IF(H118="Hard",#REF!+ 3,IF(H118="Medium",#REF!+ 7,IF(H118="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="119" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I119" t="str">
         <f>IF(H119="Hard",#REF!+ 3,IF(H119="Medium",#REF!+ 7,IF(H119="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="120" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I120" t="str">
         <f>IF(H120="Hard",#REF!+ 3,IF(H120="Medium",#REF!+ 7,IF(H120="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="121" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I121" t="str">
         <f>IF(H121="Hard",#REF!+ 3,IF(H121="Medium",#REF!+ 7,IF(H121="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="122" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I122" t="str">
         <f>IF(H122="Hard",#REF!+ 3,IF(H122="Medium",#REF!+ 7,IF(H122="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="123" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I123" t="str">
         <f>IF(H123="Hard",#REF!+ 3,IF(H123="Medium",#REF!+ 7,IF(H123="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="124" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I124" t="str">
         <f>IF(H124="Hard",#REF!+ 3,IF(H124="Medium",#REF!+ 7,IF(H124="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="125" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I125" t="str">
         <f>IF(H125="Hard",#REF!+ 3,IF(H125="Medium",#REF!+ 7,IF(H125="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="126" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I126" t="str">
         <f>IF(H126="Hard",#REF!+ 3,IF(H126="Medium",#REF!+ 7,IF(H126="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="127" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I127" t="str">
         <f>IF(H127="Hard",#REF!+ 3,IF(H127="Medium",#REF!+ 7,IF(H127="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="128" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I128" t="str">
         <f>IF(H128="Hard",#REF!+ 3,IF(H128="Medium",#REF!+ 7,IF(H128="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="129" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I129" t="str">
         <f>IF(H129="Hard",#REF!+ 3,IF(H129="Medium",#REF!+ 7,IF(H129="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="130" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I130" t="str">
         <f>IF(H130="Hard",#REF!+ 3,IF(H130="Medium",#REF!+ 7,IF(H130="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I131" t="str">
         <f>IF(H131="Hard",#REF!+ 3,IF(H131="Medium",#REF!+ 7,IF(H131="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I132" t="str">
         <f>IF(H132="Hard",#REF!+ 3,IF(H132="Medium",#REF!+ 7,IF(H132="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="133" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I133" t="str">
         <f>IF(H133="Hard",#REF!+ 3,IF(H133="Medium",#REF!+ 7,IF(H133="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="134" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I134" t="str">
         <f>IF(H134="Hard",#REF!+ 3,IF(H134="Medium",#REF!+ 7,IF(H134="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="135" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I135" t="str">
         <f>IF(H135="Hard",#REF!+ 3,IF(H135="Medium",#REF!+ 7,IF(H135="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="136" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I136" t="str">
         <f>IF(H136="Hard",#REF!+ 3,IF(H136="Medium",#REF!+ 7,IF(H136="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="137" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I137" t="str">
         <f>IF(H137="Hard",#REF!+ 3,IF(H137="Medium",#REF!+ 7,IF(H137="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="138" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I138" t="str">
         <f>IF(H138="Hard",#REF!+ 3,IF(H138="Medium",#REF!+ 7,IF(H138="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="139" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I139" t="str">
         <f>IF(H139="Hard",#REF!+ 3,IF(H139="Medium",#REF!+ 7,IF(H139="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="140" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I140" t="str">
         <f>IF(H140="Hard",#REF!+ 3,IF(H140="Medium",#REF!+ 7,IF(H140="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="141" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I141" t="str">
         <f>IF(H141="Hard",#REF!+ 3,IF(H141="Medium",#REF!+ 7,IF(H141="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="142" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I142" t="str">
         <f>IF(H142="Hard",#REF!+ 3,IF(H142="Medium",#REF!+ 7,IF(H142="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="143" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I143" t="str">
         <f>IF(H143="Hard",#REF!+ 3,IF(H143="Medium",#REF!+ 7,IF(H143="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="144" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I144" t="str">
         <f>IF(H144="Hard",#REF!+ 3,IF(H144="Medium",#REF!+ 7,IF(H144="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="145" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I145" t="str">
         <f>IF(H145="Hard",#REF!+ 3,IF(H145="Medium",#REF!+ 7,IF(H145="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="146" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I146" t="str">
         <f>IF(H146="Hard",#REF!+ 3,IF(H146="Medium",#REF!+ 7,IF(H146="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="147" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I147" t="str">
         <f>IF(H147="Hard",#REF!+ 3,IF(H147="Medium",#REF!+ 7,IF(H147="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="148" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I148" t="str">
         <f>IF(H148="Hard",#REF!+ 3,IF(H148="Medium",#REF!+ 7,IF(H148="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="149" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I149" t="str">
         <f>IF(H149="Hard",#REF!+ 3,IF(H149="Medium",#REF!+ 7,IF(H149="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="150" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I150" t="str">
         <f>IF(H150="Hard",#REF!+ 3,IF(H150="Medium",#REF!+ 7,IF(H150="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="151" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I151" t="str">
         <f>IF(H151="Hard",#REF!+ 3,IF(H151="Medium",#REF!+ 7,IF(H151="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="152" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I152" t="str">
         <f>IF(H152="Hard",#REF!+ 3,IF(H152="Medium",#REF!+ 7,IF(H152="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="153" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I153" t="str">
         <f>IF(H153="Hard",#REF!+ 3,IF(H153="Medium",#REF!+ 7,IF(H153="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="154" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I154" t="str">
         <f>IF(H154="Hard",#REF!+ 3,IF(H154="Medium",#REF!+ 7,IF(H154="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="155" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I155" t="str">
         <f>IF(H155="Hard",#REF!+ 3,IF(H155="Medium",#REF!+ 7,IF(H155="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="156" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I156" t="str">
         <f>IF(H156="Hard",#REF!+ 3,IF(H156="Medium",#REF!+ 7,IF(H156="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="157" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I157" t="str">
         <f>IF(H157="Hard",#REF!+ 3,IF(H157="Medium",#REF!+ 7,IF(H157="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="158" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I158" t="str">
         <f>IF(H158="Hard",#REF!+ 3,IF(H158="Medium",#REF!+ 7,IF(H158="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="159" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I159" t="str">
         <f>IF(H159="Hard",#REF!+ 3,IF(H159="Medium",#REF!+ 7,IF(H159="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="160" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I160" t="str">
         <f>IF(H160="Hard",#REF!+ 3,IF(H160="Medium",#REF!+ 7,IF(H160="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="161" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I161" t="str">
         <f>IF(H161="Hard",#REF!+ 3,IF(H161="Medium",#REF!+ 7,IF(H161="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="162" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I162" t="str">
         <f>IF(H162="Hard",#REF!+ 3,IF(H162="Medium",#REF!+ 7,IF(H162="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="163" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I163" t="str">
         <f>IF(H163="Hard",#REF!+ 3,IF(H163="Medium",#REF!+ 7,IF(H163="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="164" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I164" t="str">
         <f>IF(H164="Hard",#REF!+ 3,IF(H164="Medium",#REF!+ 7,IF(H164="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="165" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I165" t="str">
         <f>IF(H165="Hard",#REF!+ 3,IF(H165="Medium",#REF!+ 7,IF(H165="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="166" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I166" t="str">
         <f>IF(H166="Hard",#REF!+ 3,IF(H166="Medium",#REF!+ 7,IF(H166="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="167" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I167" t="str">
         <f>IF(H167="Hard",#REF!+ 3,IF(H167="Medium",#REF!+ 7,IF(H167="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="168" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I168" t="str">
         <f>IF(H168="Hard",#REF!+ 3,IF(H168="Medium",#REF!+ 7,IF(H168="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="169" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I169" t="str">
         <f>IF(H169="Hard",#REF!+ 3,IF(H169="Medium",#REF!+ 7,IF(H169="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="170" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I170" t="str">
         <f>IF(H170="Hard",#REF!+ 3,IF(H170="Medium",#REF!+ 7,IF(H170="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="171" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I171" t="str">
         <f>IF(H171="Hard",#REF!+ 3,IF(H171="Medium",#REF!+ 7,IF(H171="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="172" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I172" t="str">
         <f>IF(H172="Hard",#REF!+ 3,IF(H172="Medium",#REF!+ 7,IF(H172="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="173" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I173" t="str">
         <f>IF(H173="Hard",#REF!+ 3,IF(H173="Medium",#REF!+ 7,IF(H173="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="174" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I174" t="str">
         <f>IF(H174="Hard",#REF!+ 3,IF(H174="Medium",#REF!+ 7,IF(H174="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="175" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I175" t="str">
         <f>IF(H175="Hard",#REF!+ 3,IF(H175="Medium",#REF!+ 7,IF(H175="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="176" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I176" t="str">
         <f>IF(H176="Hard",#REF!+ 3,IF(H176="Medium",#REF!+ 7,IF(H176="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="177" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I177" t="str">
         <f>IF(H177="Hard",#REF!+ 3,IF(H177="Medium",#REF!+ 7,IF(H177="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="178" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I178" t="str">
         <f>IF(H178="Hard",#REF!+ 3,IF(H178="Medium",#REF!+ 7,IF(H178="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="179" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I179" t="str">
         <f>IF(H179="Hard",#REF!+ 3,IF(H179="Medium",#REF!+ 7,IF(H179="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="180" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I180" t="str">
         <f>IF(H180="Hard",#REF!+ 3,IF(H180="Medium",#REF!+ 7,IF(H180="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="181" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I181" t="str">
         <f>IF(H181="Hard",#REF!+ 3,IF(H181="Medium",#REF!+ 7,IF(H181="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I182" t="str">
         <f>IF(H182="Hard",#REF!+ 3,IF(H182="Medium",#REF!+ 7,IF(H182="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="183" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I183" t="str">
         <f>IF(H183="Hard",#REF!+ 3,IF(H183="Medium",#REF!+ 7,IF(H183="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I184" t="str">
         <f>IF(H184="Hard",#REF!+ 3,IF(H184="Medium",#REF!+ 7,IF(H184="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I185" t="str">
         <f>IF(H185="Hard",#REF!+ 3,IF(H185="Medium",#REF!+ 7,IF(H185="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I186" t="str">
         <f>IF(H186="Hard",#REF!+ 3,IF(H186="Medium",#REF!+ 7,IF(H186="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="187" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I187" t="str">
         <f>IF(H187="Hard",#REF!+ 3,IF(H187="Medium",#REF!+ 7,IF(H187="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="188" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I188" t="str">
         <f>IF(H188="Hard",#REF!+ 3,IF(H188="Medium",#REF!+ 7,IF(H188="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="189" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I189" t="str">
         <f>IF(H189="Hard",#REF!+ 3,IF(H189="Medium",#REF!+ 7,IF(H189="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="190" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I190" t="str">
         <f>IF(H190="Hard",#REF!+ 3,IF(H190="Medium",#REF!+ 7,IF(H190="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="191" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I191" t="str">
         <f>IF(H191="Hard",#REF!+ 3,IF(H191="Medium",#REF!+ 7,IF(H191="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="192" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I192" t="str">
         <f>IF(H192="Hard",#REF!+ 3,IF(H192="Medium",#REF!+ 7,IF(H192="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="193" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I193" t="str">
         <f>IF(H193="Hard",#REF!+ 3,IF(H193="Medium",#REF!+ 7,IF(H193="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="194" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I194" t="str">
         <f>IF(H194="Hard",#REF!+ 3,IF(H194="Medium",#REF!+ 7,IF(H194="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="195" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I195" t="str">
         <f>IF(H195="Hard",#REF!+ 3,IF(H195="Medium",#REF!+ 7,IF(H195="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="196" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I196" t="str">
         <f>IF(H196="Hard",#REF!+ 3,IF(H196="Medium",#REF!+ 7,IF(H196="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="197" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I197" t="str">
         <f>IF(H197="Hard",#REF!+ 3,IF(H197="Medium",#REF!+ 7,IF(H197="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="198" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I198" t="str">
         <f>IF(H198="Hard",#REF!+ 3,IF(H198="Medium",#REF!+ 7,IF(H198="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="199" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I199" t="str">
         <f>IF(H199="Hard",#REF!+ 3,IF(H199="Medium",#REF!+ 7,IF(H199="Easy",#REF!+ 30,"")))</f>
         <v/>
@@ -3597,21 +3640,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3640,7 +3683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3669,7 +3712,7 @@
         <v>46052</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3695,7 +3738,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3721,7 +3764,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3750,7 +3793,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3779,7 +3822,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3808,7 +3851,7 @@
         <v>46044</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3837,7 +3880,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3866,7 +3909,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3895,7 +3938,7 @@
         <v>46041</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3924,7 +3967,7 @@
         <v>46044</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3953,7 +3996,7 @@
         <v>46040</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3982,7 +4025,7 @@
         <v>46040</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4011,7 +4054,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4040,7 +4083,7 @@
         <v>46044</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4069,7 +4112,7 @@
         <v>46044</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4095,7 +4138,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4121,7 +4164,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4150,7 +4193,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4179,7 +4222,7 @@
         <v>46044</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4205,7 +4248,7 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4231,7 +4274,7 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4260,7 +4303,7 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4287,6 +4330,145 @@
       </c>
       <c r="I24" s="14">
         <v>46039</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" t="s">
+        <v>221</v>
+      </c>
+      <c r="G25" t="s">
+        <v>130</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I25" s="14">
+        <v>46040</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>222</v>
+      </c>
+      <c r="D26" t="s">
+        <v>223</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" t="s">
+        <v>226</v>
+      </c>
+      <c r="G26" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I26" s="14">
+        <v>46045</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>224</v>
+      </c>
+      <c r="D27" t="s">
+        <v>225</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F27" t="s">
+        <v>226</v>
+      </c>
+      <c r="G27" t="s">
+        <v>157</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I27" s="14">
+        <v>46045</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>228</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F28" t="s">
+        <v>226</v>
+      </c>
+      <c r="G28" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I28" s="14">
+        <v>46045</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>230</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" t="s">
+        <v>226</v>
+      </c>
+      <c r="G29" t="s">
+        <v>130</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I29" s="14">
+        <v>46045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code for subsets 1, 2
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44076F20-7451-4FED-AB2D-7080068F2F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2223F9D1-10CF-4D2B-94E6-A62C0D3CFC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="235">
   <si>
     <t>ID</t>
   </si>
@@ -725,6 +725,18 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/combination-sum-ii/description/</t>
+  </si>
+  <si>
+    <t>Subsets 1</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/subsets-i</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subsets-ii/</t>
+  </si>
+  <si>
+    <t>Subsets 2</t>
   </si>
 </sst>
 </file>
@@ -1172,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView topLeftCell="A32" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3640,10 +3652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3989,11 +4001,11 @@
       <c r="G12" t="s">
         <v>130</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>131</v>
+      <c r="H12" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I12" s="14">
-        <v>46040</v>
+        <v>46071</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -4018,11 +4030,11 @@
       <c r="G13" t="s">
         <v>130</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>131</v>
+      <c r="H13" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I13" s="14">
-        <v>46040</v>
+        <v>46071</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -4241,11 +4253,11 @@
       <c r="G21" t="s">
         <v>157</v>
       </c>
-      <c r="H21" s="12" t="s">
-        <v>138</v>
+      <c r="H21" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I21" s="14">
-        <v>46039</v>
+        <v>46045</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -4325,11 +4337,11 @@
       <c r="G24" t="s">
         <v>130</v>
       </c>
-      <c r="H24" s="12" t="s">
-        <v>138</v>
+      <c r="H24" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I24" s="14">
-        <v>46039</v>
+        <v>46045</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -4354,11 +4366,11 @@
       <c r="G25" t="s">
         <v>130</v>
       </c>
-      <c r="H25" s="12" t="s">
-        <v>138</v>
+      <c r="H25" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I25" s="14">
-        <v>46040</v>
+        <v>46046</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -4469,6 +4481,61 @@
       </c>
       <c r="I29" s="14">
         <v>46045</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>231</v>
+      </c>
+      <c r="D30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" t="s">
+        <v>226</v>
+      </c>
+      <c r="G30" t="s">
+        <v>157</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I30" s="14">
+        <v>46046</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C31">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
+        <v>233</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F31" t="s">
+        <v>226</v>
+      </c>
+      <c r="G31" t="s">
+        <v>130</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I31" s="14">
+        <v>46046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 2 new problems solution and updated excel sheet
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED617247-1926-48EB-A674-C3B729C75A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C558288-D051-40F7-B976-05DC45452B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA Tracker" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="239">
   <si>
     <t>ID</t>
   </si>
@@ -737,6 +737,18 @@
   </si>
   <si>
     <t>Subsets 2</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum-iii/</t>
+  </si>
+  <si>
+    <t>Combination sum 3</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/letter-combinations-of-a-phone-number/submissions/1890910877/</t>
+  </si>
+  <si>
+    <t>letter combination of a phone number</t>
   </si>
 </sst>
 </file>
@@ -1188,17 +1200,17 @@
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.54296875" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
-    <col min="6" max="6" width="33.1796875" customWidth="1"/>
-    <col min="7" max="7" width="17.54296875" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1227,7 +1239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1253,7 +1265,7 @@
         <v>46065</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1293,7 +1305,7 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1328,7 +1340,7 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1363,7 +1375,7 @@
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1398,7 +1410,7 @@
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1436,7 +1448,7 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1471,7 +1483,7 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1509,7 +1521,7 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1547,7 +1559,7 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1585,7 +1597,7 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1620,7 +1632,7 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1658,7 +1670,7 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1696,7 +1708,7 @@
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1734,7 +1746,7 @@
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1772,7 +1784,7 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1810,7 +1822,7 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1839,7 +1851,7 @@
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1871,7 +1883,7 @@
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1900,7 +1912,7 @@
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1932,7 +1944,7 @@
       <c r="Q21" s="16"/>
       <c r="R21" s="16"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1964,7 +1976,7 @@
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1993,7 +2005,7 @@
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2022,7 +2034,7 @@
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2051,7 +2063,7 @@
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2083,7 +2095,7 @@
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2115,7 +2127,7 @@
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2147,7 +2159,7 @@
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2179,7 +2191,7 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2211,7 +2223,7 @@
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2240,7 +2252,7 @@
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2272,7 +2284,7 @@
       <c r="Q32" s="16"/>
       <c r="R32" s="16"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2304,7 +2316,7 @@
       <c r="Q33" s="16"/>
       <c r="R33" s="16"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2336,7 +2348,7 @@
       <c r="Q34" s="16"/>
       <c r="R34" s="16"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2368,7 +2380,7 @@
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2391,7 +2403,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2414,7 +2426,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2437,7 +2449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2460,7 +2472,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2483,7 +2495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2506,7 +2518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2535,7 +2547,7 @@
         <v>46035</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2564,7 +2576,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2593,7 +2605,7 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2622,7 +2634,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2648,7 +2660,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2674,7 +2686,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2700,7 +2712,7 @@
         <v>46040</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2729,7 +2741,7 @@
         <v>46038</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2758,877 +2770,877 @@
         <v>46039</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I54" t="str">
         <f>IF(H54="Hard",#REF!+ 3,IF(H54="Medium",#REF!+ 7,IF(H54="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I55" t="str">
         <f>IF(H55="Hard",#REF!+ 3,IF(H55="Medium",#REF!+ 7,IF(H55="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I56" t="str">
         <f>IF(H56="Hard",#REF!+ 3,IF(H56="Medium",#REF!+ 7,IF(H56="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I57" t="str">
         <f>IF(H57="Hard",#REF!+ 3,IF(H57="Medium",#REF!+ 7,IF(H57="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I58" t="str">
         <f>IF(H58="Hard",#REF!+ 3,IF(H58="Medium",#REF!+ 7,IF(H58="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I59" t="str">
         <f>IF(H59="Hard",#REF!+ 3,IF(H59="Medium",#REF!+ 7,IF(H59="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I60" t="str">
         <f>IF(H60="Hard",#REF!+ 3,IF(H60="Medium",#REF!+ 7,IF(H60="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I61" t="str">
         <f>IF(H61="Hard",#REF!+ 3,IF(H61="Medium",#REF!+ 7,IF(H61="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I62" t="str">
         <f>IF(H62="Hard",#REF!+ 3,IF(H62="Medium",#REF!+ 7,IF(H62="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I63" t="str">
         <f>IF(H63="Hard",#REF!+ 3,IF(H63="Medium",#REF!+ 7,IF(H63="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I64" t="str">
         <f>IF(H64="Hard",#REF!+ 3,IF(H64="Medium",#REF!+ 7,IF(H64="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I65" t="str">
         <f>IF(H65="Hard",#REF!+ 3,IF(H65="Medium",#REF!+ 7,IF(H65="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I66" t="str">
         <f>IF(H66="Hard",#REF!+ 3,IF(H66="Medium",#REF!+ 7,IF(H66="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I67" t="str">
         <f>IF(H67="Hard",#REF!+ 3,IF(H67="Medium",#REF!+ 7,IF(H67="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I68" t="str">
         <f>IF(H68="Hard",#REF!+ 3,IF(H68="Medium",#REF!+ 7,IF(H68="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I69" t="str">
         <f>IF(H69="Hard",#REF!+ 3,IF(H69="Medium",#REF!+ 7,IF(H69="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I70" t="str">
         <f>IF(H70="Hard",#REF!+ 3,IF(H70="Medium",#REF!+ 7,IF(H70="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I71" t="str">
         <f>IF(H71="Hard",#REF!+ 3,IF(H71="Medium",#REF!+ 7,IF(H71="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I72" t="str">
         <f>IF(H72="Hard",#REF!+ 3,IF(H72="Medium",#REF!+ 7,IF(H72="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I73" t="str">
         <f>IF(H73="Hard",#REF!+ 3,IF(H73="Medium",#REF!+ 7,IF(H73="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I74" t="str">
         <f>IF(H74="Hard",#REF!+ 3,IF(H74="Medium",#REF!+ 7,IF(H74="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I75" t="str">
         <f>IF(H75="Hard",#REF!+ 3,IF(H75="Medium",#REF!+ 7,IF(H75="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I76" t="str">
         <f>IF(H76="Hard",#REF!+ 3,IF(H76="Medium",#REF!+ 7,IF(H76="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I77" t="str">
         <f>IF(H77="Hard",#REF!+ 3,IF(H77="Medium",#REF!+ 7,IF(H77="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I78" t="str">
         <f>IF(H78="Hard",#REF!+ 3,IF(H78="Medium",#REF!+ 7,IF(H78="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I79" t="str">
         <f>IF(H79="Hard",#REF!+ 3,IF(H79="Medium",#REF!+ 7,IF(H79="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I80" t="str">
         <f>IF(H80="Hard",#REF!+ 3,IF(H80="Medium",#REF!+ 7,IF(H80="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I81" t="str">
         <f>IF(H81="Hard",#REF!+ 3,IF(H81="Medium",#REF!+ 7,IF(H81="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I82" t="str">
         <f>IF(H82="Hard",#REF!+ 3,IF(H82="Medium",#REF!+ 7,IF(H82="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I83" t="str">
         <f>IF(H83="Hard",#REF!+ 3,IF(H83="Medium",#REF!+ 7,IF(H83="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I84" t="str">
         <f>IF(H84="Hard",#REF!+ 3,IF(H84="Medium",#REF!+ 7,IF(H84="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I85" t="str">
         <f>IF(H85="Hard",#REF!+ 3,IF(H85="Medium",#REF!+ 7,IF(H85="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I86" t="str">
         <f>IF(H86="Hard",#REF!+ 3,IF(H86="Medium",#REF!+ 7,IF(H86="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I87" t="str">
         <f>IF(H87="Hard",#REF!+ 3,IF(H87="Medium",#REF!+ 7,IF(H87="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I88" t="str">
         <f>IF(H88="Hard",#REF!+ 3,IF(H88="Medium",#REF!+ 7,IF(H88="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I89" t="str">
         <f>IF(H89="Hard",#REF!+ 3,IF(H89="Medium",#REF!+ 7,IF(H89="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I90" t="str">
         <f>IF(H90="Hard",#REF!+ 3,IF(H90="Medium",#REF!+ 7,IF(H90="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I91" t="str">
         <f>IF(H91="Hard",#REF!+ 3,IF(H91="Medium",#REF!+ 7,IF(H91="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I92" t="str">
         <f>IF(H92="Hard",#REF!+ 3,IF(H92="Medium",#REF!+ 7,IF(H92="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I93" t="str">
         <f>IF(H93="Hard",#REF!+ 3,IF(H93="Medium",#REF!+ 7,IF(H93="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I94" t="str">
         <f>IF(H94="Hard",#REF!+ 3,IF(H94="Medium",#REF!+ 7,IF(H94="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I95" t="str">
         <f>IF(H95="Hard",#REF!+ 3,IF(H95="Medium",#REF!+ 7,IF(H95="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I96" t="str">
         <f>IF(H96="Hard",#REF!+ 3,IF(H96="Medium",#REF!+ 7,IF(H96="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I97" t="str">
         <f>IF(H97="Hard",#REF!+ 3,IF(H97="Medium",#REF!+ 7,IF(H97="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I98" t="str">
         <f>IF(H98="Hard",#REF!+ 3,IF(H98="Medium",#REF!+ 7,IF(H98="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I99" t="str">
         <f>IF(H99="Hard",#REF!+ 3,IF(H99="Medium",#REF!+ 7,IF(H99="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I100" t="str">
         <f>IF(H100="Hard",#REF!+ 3,IF(H100="Medium",#REF!+ 7,IF(H100="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I101" t="str">
         <f>IF(H101="Hard",#REF!+ 3,IF(H101="Medium",#REF!+ 7,IF(H101="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I102" t="str">
         <f>IF(H102="Hard",#REF!+ 3,IF(H102="Medium",#REF!+ 7,IF(H102="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I103" t="str">
         <f>IF(H103="Hard",#REF!+ 3,IF(H103="Medium",#REF!+ 7,IF(H103="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I104" t="str">
         <f>IF(H104="Hard",#REF!+ 3,IF(H104="Medium",#REF!+ 7,IF(H104="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I105" t="str">
         <f>IF(H105="Hard",#REF!+ 3,IF(H105="Medium",#REF!+ 7,IF(H105="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I106" t="str">
         <f>IF(H106="Hard",#REF!+ 3,IF(H106="Medium",#REF!+ 7,IF(H106="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I107" t="str">
         <f>IF(H107="Hard",#REF!+ 3,IF(H107="Medium",#REF!+ 7,IF(H107="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I108" t="str">
         <f>IF(H108="Hard",#REF!+ 3,IF(H108="Medium",#REF!+ 7,IF(H108="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="109" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I109" t="str">
         <f>IF(H109="Hard",#REF!+ 3,IF(H109="Medium",#REF!+ 7,IF(H109="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="110" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I110" t="str">
         <f>IF(H110="Hard",#REF!+ 3,IF(H110="Medium",#REF!+ 7,IF(H110="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="111" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I111" t="str">
         <f>IF(H111="Hard",#REF!+ 3,IF(H111="Medium",#REF!+ 7,IF(H111="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="112" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I112" t="str">
         <f>IF(H112="Hard",#REF!+ 3,IF(H112="Medium",#REF!+ 7,IF(H112="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="113" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I113" t="str">
         <f>IF(H113="Hard",#REF!+ 3,IF(H113="Medium",#REF!+ 7,IF(H113="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="114" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I114" t="str">
         <f>IF(H114="Hard",#REF!+ 3,IF(H114="Medium",#REF!+ 7,IF(H114="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I115" t="str">
         <f>IF(H115="Hard",#REF!+ 3,IF(H115="Medium",#REF!+ 7,IF(H115="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="116" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I116" t="str">
         <f>IF(H116="Hard",#REF!+ 3,IF(H116="Medium",#REF!+ 7,IF(H116="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="117" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I117" t="str">
         <f>IF(H117="Hard",#REF!+ 3,IF(H117="Medium",#REF!+ 7,IF(H117="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="118" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I118" t="str">
         <f>IF(H118="Hard",#REF!+ 3,IF(H118="Medium",#REF!+ 7,IF(H118="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="119" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I119" t="str">
         <f>IF(H119="Hard",#REF!+ 3,IF(H119="Medium",#REF!+ 7,IF(H119="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="120" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I120" t="str">
         <f>IF(H120="Hard",#REF!+ 3,IF(H120="Medium",#REF!+ 7,IF(H120="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="121" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I121" t="str">
         <f>IF(H121="Hard",#REF!+ 3,IF(H121="Medium",#REF!+ 7,IF(H121="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="122" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I122" t="str">
         <f>IF(H122="Hard",#REF!+ 3,IF(H122="Medium",#REF!+ 7,IF(H122="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="123" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I123" t="str">
         <f>IF(H123="Hard",#REF!+ 3,IF(H123="Medium",#REF!+ 7,IF(H123="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="124" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I124" t="str">
         <f>IF(H124="Hard",#REF!+ 3,IF(H124="Medium",#REF!+ 7,IF(H124="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="125" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I125" t="str">
         <f>IF(H125="Hard",#REF!+ 3,IF(H125="Medium",#REF!+ 7,IF(H125="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="126" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I126" t="str">
         <f>IF(H126="Hard",#REF!+ 3,IF(H126="Medium",#REF!+ 7,IF(H126="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="127" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I127" t="str">
         <f>IF(H127="Hard",#REF!+ 3,IF(H127="Medium",#REF!+ 7,IF(H127="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="128" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I128" t="str">
         <f>IF(H128="Hard",#REF!+ 3,IF(H128="Medium",#REF!+ 7,IF(H128="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="129" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I129" t="str">
         <f>IF(H129="Hard",#REF!+ 3,IF(H129="Medium",#REF!+ 7,IF(H129="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="130" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I130" t="str">
         <f>IF(H130="Hard",#REF!+ 3,IF(H130="Medium",#REF!+ 7,IF(H130="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I131" t="str">
         <f>IF(H131="Hard",#REF!+ 3,IF(H131="Medium",#REF!+ 7,IF(H131="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I132" t="str">
         <f>IF(H132="Hard",#REF!+ 3,IF(H132="Medium",#REF!+ 7,IF(H132="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="133" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I133" t="str">
         <f>IF(H133="Hard",#REF!+ 3,IF(H133="Medium",#REF!+ 7,IF(H133="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="134" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I134" t="str">
         <f>IF(H134="Hard",#REF!+ 3,IF(H134="Medium",#REF!+ 7,IF(H134="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="135" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I135" t="str">
         <f>IF(H135="Hard",#REF!+ 3,IF(H135="Medium",#REF!+ 7,IF(H135="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="136" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I136" t="str">
         <f>IF(H136="Hard",#REF!+ 3,IF(H136="Medium",#REF!+ 7,IF(H136="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="137" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I137" t="str">
         <f>IF(H137="Hard",#REF!+ 3,IF(H137="Medium",#REF!+ 7,IF(H137="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="138" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I138" t="str">
         <f>IF(H138="Hard",#REF!+ 3,IF(H138="Medium",#REF!+ 7,IF(H138="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="139" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I139" t="str">
         <f>IF(H139="Hard",#REF!+ 3,IF(H139="Medium",#REF!+ 7,IF(H139="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="140" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I140" t="str">
         <f>IF(H140="Hard",#REF!+ 3,IF(H140="Medium",#REF!+ 7,IF(H140="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="141" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I141" t="str">
         <f>IF(H141="Hard",#REF!+ 3,IF(H141="Medium",#REF!+ 7,IF(H141="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="142" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I142" t="str">
         <f>IF(H142="Hard",#REF!+ 3,IF(H142="Medium",#REF!+ 7,IF(H142="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="143" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I143" t="str">
         <f>IF(H143="Hard",#REF!+ 3,IF(H143="Medium",#REF!+ 7,IF(H143="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="144" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I144" t="str">
         <f>IF(H144="Hard",#REF!+ 3,IF(H144="Medium",#REF!+ 7,IF(H144="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="145" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I145" t="str">
         <f>IF(H145="Hard",#REF!+ 3,IF(H145="Medium",#REF!+ 7,IF(H145="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="146" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I146" t="str">
         <f>IF(H146="Hard",#REF!+ 3,IF(H146="Medium",#REF!+ 7,IF(H146="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="147" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I147" t="str">
         <f>IF(H147="Hard",#REF!+ 3,IF(H147="Medium",#REF!+ 7,IF(H147="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="148" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I148" t="str">
         <f>IF(H148="Hard",#REF!+ 3,IF(H148="Medium",#REF!+ 7,IF(H148="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="149" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I149" t="str">
         <f>IF(H149="Hard",#REF!+ 3,IF(H149="Medium",#REF!+ 7,IF(H149="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="150" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I150" t="str">
         <f>IF(H150="Hard",#REF!+ 3,IF(H150="Medium",#REF!+ 7,IF(H150="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="151" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I151" t="str">
         <f>IF(H151="Hard",#REF!+ 3,IF(H151="Medium",#REF!+ 7,IF(H151="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="152" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I152" t="str">
         <f>IF(H152="Hard",#REF!+ 3,IF(H152="Medium",#REF!+ 7,IF(H152="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="153" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I153" t="str">
         <f>IF(H153="Hard",#REF!+ 3,IF(H153="Medium",#REF!+ 7,IF(H153="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="154" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I154" t="str">
         <f>IF(H154="Hard",#REF!+ 3,IF(H154="Medium",#REF!+ 7,IF(H154="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="155" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I155" t="str">
         <f>IF(H155="Hard",#REF!+ 3,IF(H155="Medium",#REF!+ 7,IF(H155="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="156" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I156" t="str">
         <f>IF(H156="Hard",#REF!+ 3,IF(H156="Medium",#REF!+ 7,IF(H156="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="157" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I157" t="str">
         <f>IF(H157="Hard",#REF!+ 3,IF(H157="Medium",#REF!+ 7,IF(H157="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="158" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I158" t="str">
         <f>IF(H158="Hard",#REF!+ 3,IF(H158="Medium",#REF!+ 7,IF(H158="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="159" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I159" t="str">
         <f>IF(H159="Hard",#REF!+ 3,IF(H159="Medium",#REF!+ 7,IF(H159="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="160" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I160" t="str">
         <f>IF(H160="Hard",#REF!+ 3,IF(H160="Medium",#REF!+ 7,IF(H160="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="161" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I161" t="str">
         <f>IF(H161="Hard",#REF!+ 3,IF(H161="Medium",#REF!+ 7,IF(H161="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="162" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="162" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I162" t="str">
         <f>IF(H162="Hard",#REF!+ 3,IF(H162="Medium",#REF!+ 7,IF(H162="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="163" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="163" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I163" t="str">
         <f>IF(H163="Hard",#REF!+ 3,IF(H163="Medium",#REF!+ 7,IF(H163="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="164" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="164" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I164" t="str">
         <f>IF(H164="Hard",#REF!+ 3,IF(H164="Medium",#REF!+ 7,IF(H164="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="165" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="165" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I165" t="str">
         <f>IF(H165="Hard",#REF!+ 3,IF(H165="Medium",#REF!+ 7,IF(H165="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="166" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="166" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I166" t="str">
         <f>IF(H166="Hard",#REF!+ 3,IF(H166="Medium",#REF!+ 7,IF(H166="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="167" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I167" t="str">
         <f>IF(H167="Hard",#REF!+ 3,IF(H167="Medium",#REF!+ 7,IF(H167="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="168" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="168" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I168" t="str">
         <f>IF(H168="Hard",#REF!+ 3,IF(H168="Medium",#REF!+ 7,IF(H168="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="169" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I169" t="str">
         <f>IF(H169="Hard",#REF!+ 3,IF(H169="Medium",#REF!+ 7,IF(H169="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="170" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="170" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I170" t="str">
         <f>IF(H170="Hard",#REF!+ 3,IF(H170="Medium",#REF!+ 7,IF(H170="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="171" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="171" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I171" t="str">
         <f>IF(H171="Hard",#REF!+ 3,IF(H171="Medium",#REF!+ 7,IF(H171="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="172" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="172" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I172" t="str">
         <f>IF(H172="Hard",#REF!+ 3,IF(H172="Medium",#REF!+ 7,IF(H172="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="173" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="173" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I173" t="str">
         <f>IF(H173="Hard",#REF!+ 3,IF(H173="Medium",#REF!+ 7,IF(H173="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="174" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="174" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I174" t="str">
         <f>IF(H174="Hard",#REF!+ 3,IF(H174="Medium",#REF!+ 7,IF(H174="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="175" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="175" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I175" t="str">
         <f>IF(H175="Hard",#REF!+ 3,IF(H175="Medium",#REF!+ 7,IF(H175="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="176" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="176" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I176" t="str">
         <f>IF(H176="Hard",#REF!+ 3,IF(H176="Medium",#REF!+ 7,IF(H176="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="177" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I177" t="str">
         <f>IF(H177="Hard",#REF!+ 3,IF(H177="Medium",#REF!+ 7,IF(H177="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="178" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I178" t="str">
         <f>IF(H178="Hard",#REF!+ 3,IF(H178="Medium",#REF!+ 7,IF(H178="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="179" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I179" t="str">
         <f>IF(H179="Hard",#REF!+ 3,IF(H179="Medium",#REF!+ 7,IF(H179="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="180" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I180" t="str">
         <f>IF(H180="Hard",#REF!+ 3,IF(H180="Medium",#REF!+ 7,IF(H180="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="181" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="181" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I181" t="str">
         <f>IF(H181="Hard",#REF!+ 3,IF(H181="Medium",#REF!+ 7,IF(H181="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="182" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I182" t="str">
         <f>IF(H182="Hard",#REF!+ 3,IF(H182="Medium",#REF!+ 7,IF(H182="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="183" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="183" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I183" t="str">
         <f>IF(H183="Hard",#REF!+ 3,IF(H183="Medium",#REF!+ 7,IF(H183="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="184" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I184" t="str">
         <f>IF(H184="Hard",#REF!+ 3,IF(H184="Medium",#REF!+ 7,IF(H184="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I185" t="str">
         <f>IF(H185="Hard",#REF!+ 3,IF(H185="Medium",#REF!+ 7,IF(H185="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="186" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I186" t="str">
         <f>IF(H186="Hard",#REF!+ 3,IF(H186="Medium",#REF!+ 7,IF(H186="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="187" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="187" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I187" t="str">
         <f>IF(H187="Hard",#REF!+ 3,IF(H187="Medium",#REF!+ 7,IF(H187="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="188" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I188" t="str">
         <f>IF(H188="Hard",#REF!+ 3,IF(H188="Medium",#REF!+ 7,IF(H188="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="189" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I189" t="str">
         <f>IF(H189="Hard",#REF!+ 3,IF(H189="Medium",#REF!+ 7,IF(H189="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="190" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I190" t="str">
         <f>IF(H190="Hard",#REF!+ 3,IF(H190="Medium",#REF!+ 7,IF(H190="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="191" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="191" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I191" t="str">
         <f>IF(H191="Hard",#REF!+ 3,IF(H191="Medium",#REF!+ 7,IF(H191="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="192" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="192" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I192" t="str">
         <f>IF(H192="Hard",#REF!+ 3,IF(H192="Medium",#REF!+ 7,IF(H192="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="193" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I193" t="str">
         <f>IF(H193="Hard",#REF!+ 3,IF(H193="Medium",#REF!+ 7,IF(H193="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="194" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="194" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I194" t="str">
         <f>IF(H194="Hard",#REF!+ 3,IF(H194="Medium",#REF!+ 7,IF(H194="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="195" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="195" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I195" t="str">
         <f>IF(H195="Hard",#REF!+ 3,IF(H195="Medium",#REF!+ 7,IF(H195="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="196" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I196" t="str">
         <f>IF(H196="Hard",#REF!+ 3,IF(H196="Medium",#REF!+ 7,IF(H196="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="197" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="197" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I197" t="str">
         <f>IF(H197="Hard",#REF!+ 3,IF(H197="Medium",#REF!+ 7,IF(H197="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="198" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="198" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I198" t="str">
         <f>IF(H198="Hard",#REF!+ 3,IF(H198="Medium",#REF!+ 7,IF(H198="Easy",#REF!+ 30,"")))</f>
         <v/>
       </c>
     </row>
-    <row r="199" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="199" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I199" t="str">
         <f>IF(H199="Hard",#REF!+ 3,IF(H199="Medium",#REF!+ 7,IF(H199="Easy",#REF!+ 30,"")))</f>
         <v/>
@@ -3652,21 +3664,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="118" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3695,7 +3707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3724,7 +3736,7 @@
         <v>46052</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3743,14 +3755,14 @@
       <c r="G3" t="s">
         <v>157</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>131</v>
+      <c r="H3" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I3" s="14">
-        <v>46041</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46072</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3769,14 +3781,14 @@
       <c r="G4" t="s">
         <v>157</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>131</v>
+      <c r="H4" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I4" s="14">
-        <v>46041</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46072</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3798,14 +3810,14 @@
       <c r="G5" t="s">
         <v>130</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>131</v>
+      <c r="H5" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I5" s="14">
-        <v>46041</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3827,14 +3839,14 @@
       <c r="G6" t="s">
         <v>130</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>131</v>
+      <c r="H6" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I6" s="14">
-        <v>46041</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46072</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3863,7 +3875,7 @@
         <v>46044</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3885,14 +3897,14 @@
       <c r="G8" t="s">
         <v>130</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>131</v>
+      <c r="H8" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I8" s="14">
-        <v>46041</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46072</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3914,14 +3926,14 @@
       <c r="G9" t="s">
         <v>130</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>131</v>
+      <c r="H9" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I9" s="14">
-        <v>46041</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3943,14 +3955,14 @@
       <c r="G10" t="s">
         <v>130</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>131</v>
+      <c r="H10" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I10" s="14">
-        <v>46041</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46072</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3979,7 +3991,7 @@
         <v>46044</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4008,7 +4020,7 @@
         <v>46071</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4037,7 +4049,7 @@
         <v>46071</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4063,10 +4075,10 @@
         <v>131</v>
       </c>
       <c r="I14" s="14">
-        <v>46042</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46048</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4095,7 +4107,7 @@
         <v>46044</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4124,7 +4136,7 @@
         <v>46044</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4147,10 +4159,10 @@
         <v>131</v>
       </c>
       <c r="I17" s="14">
-        <v>46042</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46048</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4173,10 +4185,10 @@
         <v>131</v>
       </c>
       <c r="I18" s="14">
-        <v>46042</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46048</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4202,10 +4214,10 @@
         <v>131</v>
       </c>
       <c r="I19" s="14">
-        <v>46042</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46048</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4234,7 +4246,7 @@
         <v>46044</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4260,7 +4272,7 @@
         <v>46045</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4279,14 +4291,14 @@
       <c r="G22" t="s">
         <v>157</v>
       </c>
-      <c r="H22" s="12" t="s">
-        <v>138</v>
+      <c r="H22" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I22" s="14">
-        <v>46042</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46049</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4308,14 +4320,14 @@
       <c r="G23" t="s">
         <v>130</v>
       </c>
-      <c r="H23" s="12" t="s">
-        <v>138</v>
+      <c r="H23" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I23" s="14">
-        <v>46042</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46049</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4344,7 +4356,7 @@
         <v>46045</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4373,7 +4385,7 @@
         <v>46046</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4395,14 +4407,14 @@
       <c r="G26" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="12" t="s">
-        <v>138</v>
+      <c r="H26" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I26" s="14">
-        <v>46042</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46049</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4428,7 +4440,7 @@
         <v>46046</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4454,7 +4466,7 @@
         <v>46046</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4480,7 +4492,7 @@
         <v>46046</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4509,7 +4521,7 @@
         <v>46046</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4538,7 +4550,7 @@
         <v>46046</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4564,7 +4576,7 @@
         <v>46045</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4590,7 +4602,7 @@
         <v>46045</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4619,7 +4631,7 @@
         <v>46045</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4648,7 +4660,7 @@
         <v>46045</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4674,7 +4686,7 @@
         <v>46047</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4701,6 +4713,64 @@
       </c>
       <c r="I37" s="14">
         <v>46047</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C38">
+        <v>216</v>
+      </c>
+      <c r="D38" t="s">
+        <v>235</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" t="s">
+        <v>130</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I38" s="14">
+        <v>46043</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>238</v>
+      </c>
+      <c r="C39">
+        <v>17</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F39" t="s">
+        <v>134</v>
+      </c>
+      <c r="G39" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I39" s="14">
+        <v>46043</v>
       </c>
     </row>
   </sheetData>
@@ -4717,6 +4787,7 @@
     <hyperlink ref="D27" r:id="rId10" xr:uid="{66B86A13-F07A-44A0-9C3E-ED692FCF28DD}"/>
     <hyperlink ref="D28" r:id="rId11" xr:uid="{99EC1D8B-18FF-4449-A448-68E6CD8F1060}"/>
     <hyperlink ref="D29" r:id="rId12" xr:uid="{B0F5FF3F-9639-42DF-BE99-F4910001FDEF}"/>
+    <hyperlink ref="D39" r:id="rId13" xr:uid="{0B057276-C1BD-4609-8BD8-A857B588E3F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added palindrome partitioning code and updated excel sheet
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C558288-D051-40F7-B976-05DC45452B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249090B2-3F57-4A93-A232-D702E18396ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA Tracker" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="241">
   <si>
     <t>ID</t>
   </si>
@@ -749,6 +749,12 @@
   </si>
   <si>
     <t>letter combination of a phone number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-partitioning/description/</t>
+  </si>
+  <si>
+    <t>Palindrome partioning</t>
   </si>
 </sst>
 </file>
@@ -3664,10 +3670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4737,11 +4743,11 @@
       <c r="G38" t="s">
         <v>130</v>
       </c>
-      <c r="H38" s="12" t="s">
-        <v>138</v>
+      <c r="H38" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I38" s="14">
-        <v>46043</v>
+        <v>46049</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -4766,11 +4772,40 @@
       <c r="G39" t="s">
         <v>130</v>
       </c>
-      <c r="H39" s="12" t="s">
-        <v>138</v>
+      <c r="H39" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="I39" s="14">
-        <v>46043</v>
+        <v>46049</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>240</v>
+      </c>
+      <c r="C40">
+        <v>131</v>
+      </c>
+      <c r="D40" t="s">
+        <v>239</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" t="s">
+        <v>134</v>
+      </c>
+      <c r="G40" t="s">
+        <v>130</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I40" s="14">
+        <v>46050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added word search LC Solution
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249090B2-3F57-4A93-A232-D702E18396ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039584E8-2288-4748-BCD7-1FB9BBDCEDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="243">
   <si>
     <t>ID</t>
   </si>
@@ -755,6 +755,12 @@
   </si>
   <si>
     <t>Palindrome partioning</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-search/</t>
+  </si>
+  <si>
+    <t>Word Search</t>
   </si>
 </sst>
 </file>
@@ -3670,10 +3676,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4805,6 +4811,35 @@
         <v>131</v>
       </c>
       <c r="I40" s="14">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>242</v>
+      </c>
+      <c r="C41">
+        <v>79</v>
+      </c>
+      <c r="D41" t="s">
+        <v>241</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" t="s">
+        <v>134</v>
+      </c>
+      <c r="G41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I41" s="14">
         <v>46050</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the excel sheet with revised revision dates
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DDCE4-411F-4CF8-99FA-87BCC5819F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35A7A47-BAB2-41C5-99B7-5F4AC241A50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3678,8 +3678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4390,11 +4390,11 @@
       <c r="G25" t="s">
         <v>130</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>131</v>
+      <c r="H25" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I25" s="14">
-        <v>46046</v>
+        <v>46076</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -4445,11 +4445,11 @@
       <c r="G27" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="7" t="s">
-        <v>131</v>
+      <c r="H27" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I27" s="14">
-        <v>46046</v>
+        <v>46076</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -4471,11 +4471,11 @@
       <c r="G28" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="7" t="s">
-        <v>131</v>
+      <c r="H28" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I28" s="14">
-        <v>46046</v>
+        <v>46076</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -4497,11 +4497,11 @@
       <c r="G29" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="7" t="s">
-        <v>131</v>
+      <c r="H29" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I29" s="14">
-        <v>46046</v>
+        <v>46076</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -4526,11 +4526,11 @@
       <c r="G30" t="s">
         <v>130</v>
       </c>
-      <c r="H30" s="7" t="s">
-        <v>131</v>
+      <c r="H30" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I30" s="14">
-        <v>46046</v>
+        <v>46077</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -4555,11 +4555,11 @@
       <c r="G31" t="s">
         <v>130</v>
       </c>
-      <c r="H31" s="7" t="s">
-        <v>131</v>
+      <c r="H31" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I31" s="14">
-        <v>46046</v>
+        <v>46077</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -4581,11 +4581,11 @@
       <c r="G32" t="s">
         <v>157</v>
       </c>
-      <c r="H32" s="7" t="s">
-        <v>131</v>
+      <c r="H32" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I32" s="14">
-        <v>46045</v>
+        <v>46077</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -4607,11 +4607,11 @@
       <c r="G33" t="s">
         <v>157</v>
       </c>
-      <c r="H33" s="7" t="s">
-        <v>131</v>
+      <c r="H33" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I33" s="14">
-        <v>46045</v>
+        <v>46077</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -4636,11 +4636,11 @@
       <c r="G34" t="s">
         <v>130</v>
       </c>
-      <c r="H34" s="7" t="s">
-        <v>131</v>
+      <c r="H34" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I34" s="14">
-        <v>46045</v>
+        <v>46078</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -4665,11 +4665,11 @@
       <c r="G35" t="s">
         <v>130</v>
       </c>
-      <c r="H35" s="7" t="s">
-        <v>131</v>
+      <c r="H35" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I35" s="14">
-        <v>46045</v>
+        <v>46078</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added 2 new problems solutions and updated the DSA Tracker
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625AE56C-2038-45C2-A25D-B64F5089BF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24770272-CE14-4465-A5FA-60079A2385FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="273">
   <si>
     <t>ID</t>
   </si>
@@ -827,6 +827,30 @@
   </si>
   <si>
     <t>Infix to Prefix Conversion</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/postfix-to-infix-conversion</t>
+  </si>
+  <si>
+    <t>Postfix to Infix Conversion</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/prefix-to-infix-conversion</t>
+  </si>
+  <si>
+    <t>Prefix to Infix Conversion</t>
+  </si>
+  <si>
+    <t>Postfix to prefix Conversion</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/postfix-to-prefix-conversion</t>
+  </si>
+  <si>
+    <t>Prefix to PostFix Conversion</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/prefix-to-postfix-conversion</t>
   </si>
 </sst>
 </file>
@@ -3749,10 +3773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5185,6 +5209,110 @@
         <v>150</v>
       </c>
       <c r="I51" s="14">
+        <v>46061</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>266</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F52" t="s">
+        <v>244</v>
+      </c>
+      <c r="G52" t="s">
+        <v>157</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I52" s="14">
+        <v>46061</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>268</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F53" t="s">
+        <v>244</v>
+      </c>
+      <c r="G53" t="s">
+        <v>157</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I53" s="14">
+        <v>46061</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>269</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F54" t="s">
+        <v>244</v>
+      </c>
+      <c r="G54" t="s">
+        <v>157</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I54" s="14">
+        <v>46061</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>271</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F55" t="s">
+        <v>244</v>
+      </c>
+      <c r="G55" t="s">
+        <v>157</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I55" s="14">
         <v>46061</v>
       </c>
     </row>
@@ -5210,8 +5338,12 @@
     <hyperlink ref="D49" r:id="rId18" xr:uid="{B384A6CA-F53E-4571-96A3-7612E5C77503}"/>
     <hyperlink ref="D50" r:id="rId19" xr:uid="{38CFC424-FF82-4696-A935-820767DA8636}"/>
     <hyperlink ref="D51" r:id="rId20" xr:uid="{D3D10936-8CE0-4BCC-AAFE-58669DF6DC7E}"/>
+    <hyperlink ref="D52" r:id="rId21" xr:uid="{C846ACA1-B452-4C31-B2C9-EC40FBB2E4E5}"/>
+    <hyperlink ref="D53" r:id="rId22" xr:uid="{0C7B8576-D0EE-4E43-BFA3-1FE95C00B4F6}"/>
+    <hyperlink ref="D54" r:id="rId23" xr:uid="{F3A944A4-A9C0-4229-A7C4-232DF9317209}"/>
+    <hyperlink ref="D55" r:id="rId24" xr:uid="{E1B526B3-D3BB-4B15-BDCB-4F57ADC20C8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added code for NGE 1 & NGE 2
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24770272-CE14-4465-A5FA-60079A2385FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADFD16F-265B-4990-A878-0D90166E4440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="277">
   <si>
     <t>ID</t>
   </si>
@@ -851,6 +851,18 @@
   </si>
   <si>
     <t>https://takeuforward.org/plus/dsa/problems/prefix-to-postfix-conversion</t>
+  </si>
+  <si>
+    <t>Next greater element 1</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/next-greater-element-i/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/next-greater-element-ii/editorial/</t>
+  </si>
+  <si>
+    <t>Next greater element 2</t>
   </si>
 </sst>
 </file>
@@ -3773,10 +3785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N60" sqref="N60"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60:K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5314,6 +5326,64 @@
       </c>
       <c r="I55" s="14">
         <v>46061</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>273</v>
+      </c>
+      <c r="C56">
+        <v>496</v>
+      </c>
+      <c r="D56" t="s">
+        <v>274</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F56" t="s">
+        <v>244</v>
+      </c>
+      <c r="G56" t="s">
+        <v>130</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I56" s="14">
+        <v>46069</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>276</v>
+      </c>
+      <c r="C57">
+        <v>503</v>
+      </c>
+      <c r="D57" t="s">
+        <v>275</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F57" t="s">
+        <v>244</v>
+      </c>
+      <c r="G57" t="s">
+        <v>130</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I57" s="14">
+        <v>46069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved NSE using java and updated tracker
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADFD16F-265B-4990-A878-0D90166E4440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F371A06C-A973-4531-B12E-CDA1C0DC6B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="279">
   <si>
     <t>ID</t>
   </si>
@@ -863,6 +863,12 @@
   </si>
   <si>
     <t>Next greater element 2</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/plus/dsa/problems/next-smaller-element</t>
+  </si>
+  <si>
+    <t>Next smaller element</t>
   </si>
 </sst>
 </file>
@@ -3785,10 +3791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60:K61"/>
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5384,6 +5390,32 @@
       </c>
       <c r="I57" s="14">
         <v>46069</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>278</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F58" t="s">
+        <v>244</v>
+      </c>
+      <c r="G58" t="s">
+        <v>157</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I58" s="14">
+        <v>46061</v>
       </c>
     </row>
   </sheetData>
@@ -5412,8 +5444,9 @@
     <hyperlink ref="D53" r:id="rId22" xr:uid="{0C7B8576-D0EE-4E43-BFA3-1FE95C00B4F6}"/>
     <hyperlink ref="D54" r:id="rId23" xr:uid="{F3A944A4-A9C0-4229-A7C4-232DF9317209}"/>
     <hyperlink ref="D55" r:id="rId24" xr:uid="{E1B526B3-D3BB-4B15-BDCB-4F57ADC20C8C}"/>
+    <hyperlink ref="D58" r:id="rId25" xr:uid="{FC4485FD-BE1E-4460-928B-1856C4D084ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 3 leetcode problem solutions and updated the tracker
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F371A06C-A973-4531-B12E-CDA1C0DC6B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B994DD41-9146-4BDE-907C-859CF0E572E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="285">
   <si>
     <t>ID</t>
   </si>
@@ -869,6 +869,24 @@
   </si>
   <si>
     <t>Next smaller element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/trapping-rain-water/description/</t>
+  </si>
+  <si>
+    <t>Trapping rain water</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sum-of-subarray-minimums/description/</t>
+  </si>
+  <si>
+    <t>Sum of subarray minimums</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/asteroid-collision/description/</t>
+  </si>
+  <si>
+    <t>Asteroid collision</t>
   </si>
 </sst>
 </file>
@@ -3791,10 +3809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5416,6 +5434,93 @@
       </c>
       <c r="I58" s="14">
         <v>46061</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>280</v>
+      </c>
+      <c r="C59">
+        <v>42</v>
+      </c>
+      <c r="D59" t="s">
+        <v>279</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F59" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" t="s">
+        <v>130</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I59" s="14">
+        <v>46061</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>282</v>
+      </c>
+      <c r="C60">
+        <v>907</v>
+      </c>
+      <c r="D60" t="s">
+        <v>281</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F60" t="s">
+        <v>244</v>
+      </c>
+      <c r="G60" t="s">
+        <v>130</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I60" s="14">
+        <v>46069</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>284</v>
+      </c>
+      <c r="C61">
+        <v>735</v>
+      </c>
+      <c r="D61" t="s">
+        <v>283</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F61" t="s">
+        <v>244</v>
+      </c>
+      <c r="G61" t="s">
+        <v>130</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I61" s="14">
+        <v>46069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added solution of 2 more problems from stack & updated tracker
</commit_message>
<xml_diff>
--- a/DSA_Revision_Tracker.xlsx
+++ b/DSA_Revision_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D Drive\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B994DD41-9146-4BDE-907C-859CF0E572E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE48A6A-E9D3-442A-BCEB-E3EC3A5E48A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="289">
   <si>
     <t>ID</t>
   </si>
@@ -887,6 +887,18 @@
   </si>
   <si>
     <t>Asteroid collision</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sum-of-subarray-ranges/description/</t>
+  </si>
+  <si>
+    <t>Sum of subarray ranges</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-k-digits/description/</t>
+  </si>
+  <si>
+    <t>Remove k digits</t>
   </si>
 </sst>
 </file>
@@ -3809,10 +3821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B45570-3751-416D-AB72-9ED524E7000B}">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M70" sqref="M70"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5520,6 +5532,64 @@
         <v>131</v>
       </c>
       <c r="I61" s="14">
+        <v>46069</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>286</v>
+      </c>
+      <c r="C62">
+        <v>2104</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F62" t="s">
+        <v>244</v>
+      </c>
+      <c r="G62" t="s">
+        <v>130</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I62" s="14">
+        <v>46069</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>288</v>
+      </c>
+      <c r="C63">
+        <v>402</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F63" t="s">
+        <v>244</v>
+      </c>
+      <c r="G63" t="s">
+        <v>130</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I63" s="14">
         <v>46069</v>
       </c>
     </row>
@@ -5550,8 +5620,10 @@
     <hyperlink ref="D54" r:id="rId23" xr:uid="{F3A944A4-A9C0-4229-A7C4-232DF9317209}"/>
     <hyperlink ref="D55" r:id="rId24" xr:uid="{E1B526B3-D3BB-4B15-BDCB-4F57ADC20C8C}"/>
     <hyperlink ref="D58" r:id="rId25" xr:uid="{FC4485FD-BE1E-4460-928B-1856C4D084ED}"/>
+    <hyperlink ref="D63" r:id="rId26" xr:uid="{FC0E5B1F-C938-40F3-A07A-24D21435800B}"/>
+    <hyperlink ref="D62" r:id="rId27" xr:uid="{669ECA50-18B5-4468-85AB-1AFED704AA8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>